<commit_message>
Added ability to write BEP to CTI files in OpenMKM.
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\omkm_io\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1566A6-8DAD-4927-8CAE-D77F5AAC94F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35944FF7-8E07-45E1-B7D3-FDD62FF3A6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24324" yWindow="1056" windowWidth="21600" windowHeight="11388" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="576" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
     <sheet name="species" sheetId="1" r:id="rId2"/>
-    <sheet name="phases" sheetId="5" r:id="rId3"/>
-    <sheet name="reactions" sheetId="3" r:id="rId4"/>
-    <sheet name="lateral_interactions" sheetId="6" r:id="rId5"/>
+    <sheet name="beps" sheetId="7" r:id="rId3"/>
+    <sheet name="phases" sheetId="5" r:id="rId4"/>
+    <sheet name="reactions" sheetId="3" r:id="rId5"/>
+    <sheet name="lateral_interactions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -181,15 +182,6 @@
     <t>RU(S)</t>
   </si>
   <si>
-    <t>NH3(S) + RU(S)= TS1_NH3(S) = NH2(S) + H(S) + RU(B)</t>
-  </si>
-  <si>
-    <t>NH2(S) + RU(S) = TS2_NH2(S) = NH(S)  + H(S) + RU(B)</t>
-  </si>
-  <si>
-    <t>NH(S)  + RU(S) = TS3_NH(S) = N(S)   + H(S) + RU(B)</t>
-  </si>
-  <si>
     <t>2N(S) + RU(B) = TS4_N2(S) = N2(S)  +  RU(S)</t>
   </si>
   <si>
@@ -299,6 +291,129 @@
   </si>
   <si>
     <t>Slopes (in kcal/mol) to use between the intervals</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Optional name to give to reaction</t>
+  </si>
+  <si>
+    <t>N-H</t>
+  </si>
+  <si>
+    <t>NH-H</t>
+  </si>
+  <si>
+    <t>NH2-H</t>
+  </si>
+  <si>
+    <t>Slope of BEP relationship</t>
+  </si>
+  <si>
+    <t>Intercept of BEP relationship in kcal/mol</t>
+  </si>
+  <si>
+    <t>cleavage</t>
+  </si>
+  <si>
+    <t>Used for BEP relationships. The direction of the elementary step. Supported options are 'synthesis' or 'cleavage'.</t>
+  </si>
+  <si>
+    <t>Direction of BEP relationship. Supported options are 'synthesis' or 'cleavage'.</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Values taken from https://github.com/VlachosGroup/NH3-Matlab-Microkinetic-Model/blob/master/amm_BEP_LSR.m#L79</t>
+  </si>
+  <si>
+    <t>Values taken from https://github.com/VlachosGroup/NH3-Matlab-Microkinetic-Model/blob/master/amm_BEP_LSR.m#L80</t>
+  </si>
+  <si>
+    <t>Values taken from https://github.com/VlachosGroup/NH3-Matlab-Microkinetic-Model/blob/master/amm_BEP_LSR.m#L81</t>
+  </si>
+  <si>
+    <t>NH3(S) + RU(S)= NH2-H = NH2(S) + H(S) + RU(B)</t>
+  </si>
+  <si>
+    <t>NH2(S) + RU(S) = NH-H = NH(S)  + H(S) + RU(B)</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>N2(T)</t>
+  </si>
+  <si>
+    <t>N(T)</t>
+  </si>
+  <si>
+    <t>H(T)</t>
+  </si>
+  <si>
+    <t>NH3(T)</t>
+  </si>
+  <si>
+    <t>NH2(T)</t>
+  </si>
+  <si>
+    <t>NH(T)</t>
+  </si>
+  <si>
+    <t>TS1_NH3(T)</t>
+  </si>
+  <si>
+    <t>TS2_NH2(T)</t>
+  </si>
+  <si>
+    <t>TS3_NH(T)</t>
+  </si>
+  <si>
+    <t>TS4_N2(T)</t>
+  </si>
+  <si>
+    <t>RU(T)</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>H2 + 2RU(T) = 2H(T) + 2RU(B)</t>
+  </si>
+  <si>
+    <t>N2 + RU(T)  = N2(T) + RU(B)</t>
+  </si>
+  <si>
+    <t>NH3 + RU(T) = NH3(T) + RU(B)</t>
+  </si>
+  <si>
+    <t>NH3(T) + RU(T)= NH2-H = NH2(T) + H(T) + RU(B)</t>
+  </si>
+  <si>
+    <t>NH2(T) + RU(T) = NH-H = NH(T)  + H(T) + RU(B)</t>
+  </si>
+  <si>
+    <t>NH(T)  + RU(T) = N-H = N(T)   + H(T) + RU(B)</t>
+  </si>
+  <si>
+    <t>2N(T) + RU(B) = TS4_N2(T) = N2(T)  +  RU(T)</t>
+  </si>
+  <si>
+    <t>synthesis</t>
+  </si>
+  <si>
+    <t>N(S) + H(S) + RU(B) = N-H = NH(S)  + RU(S)</t>
   </si>
 </sst>
 </file>
@@ -801,7 +916,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -815,6 +930,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1177,7 +1294,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1227,16 +1344,16 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1442,7 +1559,7 @@
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1678,13 +1795,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR60"/>
+  <dimension ref="A1:BR63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1827,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1728,40 +1845,40 @@
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -1817,19 +1934,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>16</v>
@@ -1933,7 +2050,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -2021,7 +2138,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -2112,7 +2229,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -2191,13 +2308,13 @@
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -2280,13 +2397,13 @@
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
@@ -2365,13 +2482,13 @@
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
@@ -2435,7 +2552,7 @@
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2444,7 +2561,7 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -2526,7 +2643,7 @@
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2535,7 +2652,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
@@ -2611,7 +2728,7 @@
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2620,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
@@ -2690,7 +2807,7 @@
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2777,7 +2894,7 @@
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2858,7 +2975,7 @@
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2933,7 +3050,7 @@
     </row>
     <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3005,13 +3122,13 @@
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -3067,31 +3184,45 @@
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4">
+        <v>-17.389999999999986</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1015.734101</v>
+      </c>
+      <c r="K17" s="4">
+        <v>456.07363700000002</v>
+      </c>
+      <c r="L17" s="4">
+        <v>408.12729300000001</v>
+      </c>
+      <c r="M17" s="4">
+        <v>378.51690000000002</v>
+      </c>
+      <c r="N17" s="4">
+        <v>344.87134400000002</v>
+      </c>
+      <c r="O17" s="4">
+        <v>334.62168200000002</v>
+      </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
-      <c r="V17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
@@ -3128,7 +3259,40 @@
       <c r="BR17" s="1"/>
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4">
+        <v>-9.3899999999999864</v>
+      </c>
+      <c r="J18" s="4">
+        <v>529.80737599999998</v>
+      </c>
+      <c r="K18" s="4">
+        <v>506.95443399999999</v>
+      </c>
+      <c r="L18" s="4">
+        <v>471.09772600000002</v>
+      </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
@@ -3165,7 +3329,40 @@
       <c r="BR18" s="1"/>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4">
+        <v>-4</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1003.51</v>
+      </c>
+      <c r="K19" s="4">
+        <v>625.54999999999995</v>
+      </c>
+      <c r="L19" s="4">
+        <v>616.29</v>
+      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
@@ -3202,7 +3399,61 @@
       <c r="BR19" s="1"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4">
+        <v>-20.67999999999995</v>
+      </c>
+      <c r="J20" s="4">
+        <v>3498.0269910000002</v>
+      </c>
+      <c r="K20" s="4">
+        <v>3469.3304969999999</v>
+      </c>
+      <c r="L20" s="4">
+        <v>3362.813486</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1590.9105280000001</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1579.266171</v>
+      </c>
+      <c r="O20" s="4">
+        <v>1140.7628299999999</v>
+      </c>
+      <c r="P20" s="4">
+        <v>564.97479799999996</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>555.49956799999995</v>
+      </c>
+      <c r="R20" s="4">
+        <v>336.10022600000002</v>
+      </c>
+      <c r="S20" s="4">
+        <v>117.161717</v>
+      </c>
+      <c r="T20" s="4">
+        <v>86.774373999999995</v>
+      </c>
+      <c r="U20" s="4">
+        <v>78.100128999999995</v>
+      </c>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="1"/>
@@ -3239,7 +3490,55 @@
       <c r="BR20" s="1"/>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4">
+        <v>-17.149999999999977</v>
+      </c>
+      <c r="J21" s="4">
+        <v>3528.6824689999999</v>
+      </c>
+      <c r="K21" s="4">
+        <v>3375.447388</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1477.164</v>
+      </c>
+      <c r="M21" s="4">
+        <v>720.07573000000002</v>
+      </c>
+      <c r="N21" s="4">
+        <v>615.66630499999997</v>
+      </c>
+      <c r="O21" s="4">
+        <v>581.96669099999997</v>
+      </c>
+      <c r="P21" s="4">
+        <v>468.85326900000001</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>286.369823</v>
+      </c>
+      <c r="R21" s="4">
+        <v>105.95658400000001</v>
+      </c>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
@@ -3276,7 +3575,49 @@
       <c r="BR21" s="1"/>
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4">
+        <v>-13.1099999999999</v>
+      </c>
+      <c r="J22" s="4">
+        <v>3384.3746510000001</v>
+      </c>
+      <c r="K22" s="4">
+        <v>726.230954</v>
+      </c>
+      <c r="L22" s="4">
+        <v>669.42910800000004</v>
+      </c>
+      <c r="M22" s="4">
+        <v>506.27813500000002</v>
+      </c>
+      <c r="N22" s="4">
+        <v>409.50201399999997</v>
+      </c>
+      <c r="O22" s="4">
+        <v>387.80818099999999</v>
+      </c>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
@@ -3313,7 +3654,57 @@
       <c r="BR22" s="1"/>
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4">
+        <v>-19.809999999999945</v>
+      </c>
+      <c r="J23" s="4">
+        <v>3484.3961949999998</v>
+      </c>
+      <c r="K23" s="4">
+        <v>3385.2659090000002</v>
+      </c>
+      <c r="L23" s="4">
+        <v>1685.8293080000001</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1480.998257</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1002.067555</v>
+      </c>
+      <c r="O23" s="4">
+        <v>916.14745100000005</v>
+      </c>
+      <c r="P23" s="4">
+        <v>575.40527899999995</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>431.30664400000001</v>
+      </c>
+      <c r="R23" s="4">
+        <v>345.148708</v>
+      </c>
+      <c r="S23" s="4">
+        <v>221.64965799999999</v>
+      </c>
+      <c r="T23" s="4">
+        <v>70.339661000000007</v>
+      </c>
+      <c r="U23" s="4"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
       <c r="AL23" s="1"/>
@@ -3350,7 +3741,51 @@
       <c r="BR23" s="1"/>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4">
+        <v>-15.819999999999936</v>
+      </c>
+      <c r="J24" s="4">
+        <v>3432.815967</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1789.8865699999999</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1032.1897269999999</v>
+      </c>
+      <c r="M24" s="4">
+        <v>583.47939799999995</v>
+      </c>
+      <c r="N24" s="4">
+        <v>392.83707299999998</v>
+      </c>
+      <c r="O24" s="4">
+        <v>384.833597</v>
+      </c>
+      <c r="P24" s="4">
+        <v>311.60087600000003</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>110.96862400000001</v>
+      </c>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
@@ -3387,7 +3822,45 @@
       <c r="BR24" s="1"/>
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4">
+        <v>-12.120000000000005</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1679.786106</v>
+      </c>
+      <c r="K25" s="4">
+        <v>509.64356400000003</v>
+      </c>
+      <c r="L25" s="4">
+        <v>489.064573</v>
+      </c>
+      <c r="M25" s="4">
+        <v>443.45080000000002</v>
+      </c>
+      <c r="N25" s="4">
+        <v>396.19289099999997</v>
+      </c>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
@@ -3424,7 +3897,42 @@
       <c r="BR25" s="1"/>
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4">
+        <v>-16.799999999999955</v>
+      </c>
+      <c r="J26" s="4">
+        <v>549.17255799999998</v>
+      </c>
+      <c r="K26" s="4">
+        <v>496.630066</v>
+      </c>
+      <c r="L26" s="4">
+        <v>436.16551199999998</v>
+      </c>
+      <c r="M26" s="4">
+        <v>418.36746199999999</v>
+      </c>
+      <c r="N26" s="4">
+        <v>391.94338199999999</v>
+      </c>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
@@ -3461,7 +3969,32 @@
       <c r="BR26" s="1"/>
     </row>
     <row r="27" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
@@ -3498,7 +4031,32 @@
       <c r="BR27" s="1"/>
     </row>
     <row r="28" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="E28" s="1"/>
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="1"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
@@ -4718,6 +5276,117 @@
       <c r="BQ60" s="1"/>
       <c r="BR60" s="1"/>
     </row>
+    <row r="61" spans="5:70" x14ac:dyDescent="0.25">
+      <c r="E61" s="1"/>
+      <c r="AJ61" s="1"/>
+      <c r="AK61" s="1"/>
+      <c r="AL61" s="1"/>
+      <c r="AM61" s="1"/>
+      <c r="AN61" s="1"/>
+      <c r="AO61" s="1"/>
+      <c r="AP61" s="1"/>
+      <c r="AQ61" s="1"/>
+      <c r="AR61" s="1"/>
+      <c r="AS61" s="1"/>
+      <c r="AT61" s="1"/>
+      <c r="AU61" s="1"/>
+      <c r="AV61" s="1"/>
+      <c r="AW61" s="1"/>
+      <c r="AX61" s="1"/>
+      <c r="AY61" s="1"/>
+      <c r="AZ61" s="1"/>
+      <c r="BA61" s="1"/>
+      <c r="BB61" s="1"/>
+      <c r="BC61" s="1"/>
+      <c r="BD61" s="1"/>
+      <c r="BE61" s="1"/>
+      <c r="BF61" s="1"/>
+      <c r="BG61" s="1"/>
+      <c r="BI61" s="1"/>
+      <c r="BJ61" s="1"/>
+      <c r="BK61" s="1"/>
+      <c r="BL61" s="1"/>
+      <c r="BM61" s="1"/>
+      <c r="BN61" s="1"/>
+      <c r="BO61" s="1"/>
+      <c r="BP61" s="1"/>
+      <c r="BQ61" s="1"/>
+      <c r="BR61" s="1"/>
+    </row>
+    <row r="62" spans="5:70" x14ac:dyDescent="0.25">
+      <c r="E62" s="1"/>
+      <c r="AJ62" s="1"/>
+      <c r="AK62" s="1"/>
+      <c r="AL62" s="1"/>
+      <c r="AM62" s="1"/>
+      <c r="AN62" s="1"/>
+      <c r="AO62" s="1"/>
+      <c r="AP62" s="1"/>
+      <c r="AQ62" s="1"/>
+      <c r="AR62" s="1"/>
+      <c r="AS62" s="1"/>
+      <c r="AT62" s="1"/>
+      <c r="AU62" s="1"/>
+      <c r="AV62" s="1"/>
+      <c r="AW62" s="1"/>
+      <c r="AX62" s="1"/>
+      <c r="AY62" s="1"/>
+      <c r="AZ62" s="1"/>
+      <c r="BA62" s="1"/>
+      <c r="BB62" s="1"/>
+      <c r="BC62" s="1"/>
+      <c r="BD62" s="1"/>
+      <c r="BE62" s="1"/>
+      <c r="BF62" s="1"/>
+      <c r="BG62" s="1"/>
+      <c r="BI62" s="1"/>
+      <c r="BJ62" s="1"/>
+      <c r="BK62" s="1"/>
+      <c r="BL62" s="1"/>
+      <c r="BM62" s="1"/>
+      <c r="BN62" s="1"/>
+      <c r="BO62" s="1"/>
+      <c r="BP62" s="1"/>
+      <c r="BQ62" s="1"/>
+      <c r="BR62" s="1"/>
+    </row>
+    <row r="63" spans="5:70" x14ac:dyDescent="0.25">
+      <c r="E63" s="1"/>
+      <c r="AJ63" s="1"/>
+      <c r="AK63" s="1"/>
+      <c r="AL63" s="1"/>
+      <c r="AM63" s="1"/>
+      <c r="AN63" s="1"/>
+      <c r="AO63" s="1"/>
+      <c r="AP63" s="1"/>
+      <c r="AQ63" s="1"/>
+      <c r="AR63" s="1"/>
+      <c r="AS63" s="1"/>
+      <c r="AT63" s="1"/>
+      <c r="AU63" s="1"/>
+      <c r="AV63" s="1"/>
+      <c r="AW63" s="1"/>
+      <c r="AX63" s="1"/>
+      <c r="AY63" s="1"/>
+      <c r="AZ63" s="1"/>
+      <c r="BA63" s="1"/>
+      <c r="BB63" s="1"/>
+      <c r="BC63" s="1"/>
+      <c r="BD63" s="1"/>
+      <c r="BE63" s="1"/>
+      <c r="BF63" s="1"/>
+      <c r="BG63" s="1"/>
+      <c r="BI63" s="1"/>
+      <c r="BJ63" s="1"/>
+      <c r="BK63" s="1"/>
+      <c r="BL63" s="1"/>
+      <c r="BM63" s="1"/>
+      <c r="BN63" s="1"/>
+      <c r="BO63" s="1"/>
+      <c r="BP63" s="1"/>
+      <c r="BQ63" s="1"/>
+      <c r="BR63" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4725,14 +5394,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA3BA1A-334E-44D2-96CB-219546C8DBF5}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C3">
+        <v>23.23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>0.52</v>
+      </c>
+      <c r="C4">
+        <v>19.78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>0.71</v>
+      </c>
+      <c r="C5">
+        <v>23.69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4742,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>43</v>
@@ -4751,49 +5518,49 @@
         <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -4801,42 +5568,68 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>12.4</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D5" s="8">
         <v>2.1671000000000001E-9</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>71</v>
+      <c r="D6" s="8">
+        <v>4.4385000000000002E-10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4845,15 +5638,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4861,127 +5654,230 @@
     <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
         <v>81</v>
-      </c>
-      <c r="B1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -4992,10 +5888,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5006,10 +5902,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5020,10 +5916,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5034,15 +5930,85 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
+        <v>-20.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-52.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-17.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-17.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>-20.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more robust CTI writer for OpenMKM
IDs are now automatically assigned to reactions and lateral interactions if not assigned previously.

Ranges in CTI writer (e.g. '0001 to 0010') is now more robust. It can group arbitrary IDs as long as they are in the form <header><delimiter><numerical ID>.
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35944FF7-8E07-45E1-B7D3-FDD62FF3A6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C80BA7-DAD5-401B-B531-02A650CBF8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="576" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="121">
   <si>
     <t>name</t>
   </si>
@@ -221,21 +221,6 @@
     <t>Type of phase</t>
   </si>
   <si>
-    <t>reactions</t>
-  </si>
-  <si>
-    <t>interactions</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>Write 'all' if reactions will occur on this phase. Tends to be true for InteractingPhase</t>
-  </si>
-  <si>
-    <t>Write 'all' if lateral interactions are present on this phase. Tends to be true for InteractingPhase</t>
-  </si>
-  <si>
     <t>InteractingInterface</t>
   </si>
   <si>
@@ -348,9 +333,6 @@
   </si>
   <si>
     <t>NH2(S) + RU(S) = NH-H = NH(S)  + H(S) + RU(B)</t>
-  </si>
-  <si>
-    <t>0001</t>
   </si>
   <si>
     <t>N2(T)</t>
@@ -1297,22 +1279,22 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1305,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1398,7 +1380,7 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1443,7 +1425,7 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1478,7 +1460,7 @@
         <v>2744</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1522,7 +1504,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1557,9 +1539,9 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1581,7 +1563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1590,7 +1572,7 @@
       <c r="G7" s="3"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1599,7 +1581,7 @@
       <c r="G8" s="3"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1608,7 +1590,7 @@
       <c r="G9" s="3"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1617,7 +1599,7 @@
       <c r="G10" s="3"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1626,7 +1608,7 @@
       <c r="G11" s="3"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1635,7 +1617,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1644,7 +1626,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1653,7 +1635,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1662,7 +1644,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1671,7 +1653,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1680,7 +1662,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1689,7 +1671,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1698,7 +1680,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1707,7 +1689,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1716,7 +1698,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1725,7 +1707,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1734,7 +1716,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1743,7 +1725,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1752,7 +1734,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1761,7 +1743,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1770,7 +1752,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1779,7 +1761,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1804,19 +1786,19 @@
       <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1809,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1929,18 +1911,18 @@
       <c r="BQ1" s="1"/>
       <c r="BR1" s="1"/>
     </row>
-    <row r="2" spans="1:70" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>55</v>
@@ -2042,7 +2024,7 @@
       <c r="BQ2" s="1"/>
       <c r="BR2" s="1"/>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2127,7 +2109,7 @@
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2221,7 +2203,7 @@
       <c r="BQ4" s="1"/>
       <c r="BR4" s="1"/>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2306,9 +2288,9 @@
       <c r="BQ5" s="1"/>
       <c r="BR5" s="1"/>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2395,9 +2377,9 @@
       <c r="BQ6" s="1"/>
       <c r="BR6" s="1"/>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2480,9 +2462,9 @@
       <c r="BQ7" s="1"/>
       <c r="BR7" s="1"/>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2550,9 +2532,9 @@
       <c r="BQ8" s="1"/>
       <c r="BR8" s="1"/>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2641,9 +2623,9 @@
       <c r="BQ9" s="1"/>
       <c r="BR9" s="1"/>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2726,9 +2708,9 @@
       <c r="BQ10" s="1"/>
       <c r="BR10" s="1"/>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2805,9 +2787,9 @@
       <c r="BQ11" s="1"/>
       <c r="BR11" s="1"/>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2892,9 +2874,9 @@
       <c r="BQ12" s="1"/>
       <c r="BR12" s="1"/>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2973,9 +2955,9 @@
       <c r="BQ13" s="1"/>
       <c r="BR13" s="1"/>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3048,9 +3030,9 @@
       <c r="BQ14" s="1"/>
       <c r="BR14" s="1"/>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3120,9 +3102,9 @@
       <c r="BP15" s="1"/>
       <c r="BQ15" s="1"/>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3182,7 +3164,7 @@
       <c r="BQ16" s="1"/>
       <c r="BR16" s="1"/>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3190,7 +3172,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
         <v>3</v>
@@ -3258,7 +3240,7 @@
       <c r="BQ17" s="1"/>
       <c r="BR17" s="1"/>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3266,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F18" t="s">
         <v>3</v>
@@ -3328,7 +3310,7 @@
       <c r="BQ18" s="1"/>
       <c r="BR18" s="1"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -3336,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -3398,7 +3380,7 @@
       <c r="BQ19" s="1"/>
       <c r="BR19" s="1"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3409,7 +3391,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
         <v>3</v>
@@ -3489,7 +3471,7 @@
       <c r="BQ20" s="1"/>
       <c r="BR20" s="1"/>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -3500,7 +3482,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F21" t="s">
         <v>3</v>
@@ -3574,7 +3556,7 @@
       <c r="BQ21" s="1"/>
       <c r="BR21" s="1"/>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -3585,7 +3567,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -3653,7 +3635,7 @@
       <c r="BQ22" s="1"/>
       <c r="BR22" s="1"/>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3740,7 +3722,7 @@
       <c r="BQ23" s="1"/>
       <c r="BR23" s="1"/>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3821,7 +3803,7 @@
       <c r="BQ24" s="1"/>
       <c r="BR24" s="1"/>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -3896,7 +3878,7 @@
       <c r="BQ25" s="1"/>
       <c r="BR25" s="1"/>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3968,7 +3950,7 @@
       <c r="BQ26" s="1"/>
       <c r="BR26" s="1"/>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -3976,7 +3958,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
         <v>24</v>
@@ -4030,7 +4012,7 @@
       <c r="BQ27" s="1"/>
       <c r="BR27" s="1"/>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4092,7 +4074,7 @@
       <c r="BQ28" s="1"/>
       <c r="BR28" s="1"/>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
       <c r="E29" s="1"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
@@ -4129,7 +4111,7 @@
       <c r="BQ29" s="1"/>
       <c r="BR29" s="1"/>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
@@ -4166,7 +4148,7 @@
       <c r="BQ30" s="1"/>
       <c r="BR30" s="1"/>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
@@ -4203,7 +4185,7 @@
       <c r="BQ31" s="1"/>
       <c r="BR31" s="1"/>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
@@ -4240,7 +4222,7 @@
       <c r="BQ32" s="1"/>
       <c r="BR32" s="1"/>
     </row>
-    <row r="33" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
@@ -4277,7 +4259,7 @@
       <c r="BQ33" s="1"/>
       <c r="BR33" s="1"/>
     </row>
-    <row r="34" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
@@ -4314,7 +4296,7 @@
       <c r="BQ34" s="1"/>
       <c r="BR34" s="1"/>
     </row>
-    <row r="35" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
@@ -4351,7 +4333,7 @@
       <c r="BQ35" s="1"/>
       <c r="BR35" s="1"/>
     </row>
-    <row r="36" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
@@ -4388,7 +4370,7 @@
       <c r="BQ36" s="1"/>
       <c r="BR36" s="1"/>
     </row>
-    <row r="37" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
@@ -4425,7 +4407,7 @@
       <c r="BQ37" s="1"/>
       <c r="BR37" s="1"/>
     </row>
-    <row r="38" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
@@ -4462,7 +4444,7 @@
       <c r="BQ38" s="1"/>
       <c r="BR38" s="1"/>
     </row>
-    <row r="39" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E39" s="1"/>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
@@ -4499,7 +4481,7 @@
       <c r="BQ39" s="1"/>
       <c r="BR39" s="1"/>
     </row>
-    <row r="40" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
@@ -4536,7 +4518,7 @@
       <c r="BQ40" s="1"/>
       <c r="BR40" s="1"/>
     </row>
-    <row r="41" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E41" s="1"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
@@ -4573,7 +4555,7 @@
       <c r="BQ41" s="1"/>
       <c r="BR41" s="1"/>
     </row>
-    <row r="42" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E42" s="1"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
@@ -4610,7 +4592,7 @@
       <c r="BQ42" s="1"/>
       <c r="BR42" s="1"/>
     </row>
-    <row r="43" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E43" s="1"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
@@ -4647,7 +4629,7 @@
       <c r="BQ43" s="1"/>
       <c r="BR43" s="1"/>
     </row>
-    <row r="44" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E44" s="1"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
@@ -4684,7 +4666,7 @@
       <c r="BQ44" s="1"/>
       <c r="BR44" s="1"/>
     </row>
-    <row r="45" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E45" s="1"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
@@ -4721,7 +4703,7 @@
       <c r="BQ45" s="1"/>
       <c r="BR45" s="1"/>
     </row>
-    <row r="46" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E46" s="1"/>
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
@@ -4758,7 +4740,7 @@
       <c r="BQ46" s="1"/>
       <c r="BR46" s="1"/>
     </row>
-    <row r="47" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E47" s="1"/>
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
@@ -4795,7 +4777,7 @@
       <c r="BQ47" s="1"/>
       <c r="BR47" s="1"/>
     </row>
-    <row r="48" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E48" s="1"/>
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
@@ -4832,7 +4814,7 @@
       <c r="BQ48" s="1"/>
       <c r="BR48" s="1"/>
     </row>
-    <row r="49" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E49" s="1"/>
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
@@ -4869,7 +4851,7 @@
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
     </row>
-    <row r="50" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E50" s="1"/>
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
@@ -4906,7 +4888,7 @@
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
     </row>
-    <row r="51" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E51" s="1"/>
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
@@ -4943,7 +4925,7 @@
       <c r="BQ51" s="1"/>
       <c r="BR51" s="1"/>
     </row>
-    <row r="52" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E52" s="1"/>
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
@@ -4980,7 +4962,7 @@
       <c r="BQ52" s="1"/>
       <c r="BR52" s="1"/>
     </row>
-    <row r="53" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E53" s="1"/>
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
@@ -5017,7 +4999,7 @@
       <c r="BQ53" s="1"/>
       <c r="BR53" s="1"/>
     </row>
-    <row r="54" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E54" s="1"/>
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
@@ -5054,7 +5036,7 @@
       <c r="BQ54" s="1"/>
       <c r="BR54" s="1"/>
     </row>
-    <row r="55" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E55" s="1"/>
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
@@ -5091,7 +5073,7 @@
       <c r="BQ55" s="1"/>
       <c r="BR55" s="1"/>
     </row>
-    <row r="56" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E56" s="1"/>
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
@@ -5128,7 +5110,7 @@
       <c r="BQ56" s="1"/>
       <c r="BR56" s="1"/>
     </row>
-    <row r="57" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E57" s="1"/>
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
@@ -5165,7 +5147,7 @@
       <c r="BQ57" s="1"/>
       <c r="BR57" s="1"/>
     </row>
-    <row r="58" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E58" s="1"/>
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
@@ -5202,7 +5184,7 @@
       <c r="BQ58" s="1"/>
       <c r="BR58" s="1"/>
     </row>
-    <row r="59" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E59" s="1"/>
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
@@ -5239,7 +5221,7 @@
       <c r="BQ59" s="1"/>
       <c r="BR59" s="1"/>
     </row>
-    <row r="60" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E60" s="1"/>
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
@@ -5276,7 +5258,7 @@
       <c r="BQ60" s="1"/>
       <c r="BR60" s="1"/>
     </row>
-    <row r="61" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E61" s="1"/>
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
@@ -5313,7 +5295,7 @@
       <c r="BQ61" s="1"/>
       <c r="BR61" s="1"/>
     </row>
-    <row r="62" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E62" s="1"/>
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
@@ -5350,7 +5332,7 @@
       <c r="BQ62" s="1"/>
       <c r="BR62" s="1"/>
     </row>
-    <row r="63" spans="5:70" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:70" x14ac:dyDescent="0.3">
       <c r="E63" s="1"/>
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
@@ -5404,40 +5386,40 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>0.28999999999999998</v>
@@ -5446,15 +5428,15 @@
         <v>23.23</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>0.52</v>
@@ -5463,15 +5445,15 @@
         <v>19.78</v>
       </c>
       <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
         <v>96</v>
       </c>
-      <c r="E4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <v>0.71</v>
@@ -5480,10 +5462,10 @@
         <v>23.69</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -5493,23 +5475,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>43</v>
@@ -5518,22 +5500,16 @@
         <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -5546,19 +5522,13 @@
       <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -5566,70 +5536,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>12.4</v>
       </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" s="8">
         <v>2.1671000000000001E-9</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>64</v>
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D6" s="8">
         <v>4.4385000000000002E-10</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>64</v>
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -5642,19 +5600,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -5662,13 +5620,13 @@
         <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5676,87 +5634,85 @@
         <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -5765,7 +5721,7 @@
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -5774,7 +5730,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -5783,43 +5739,43 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -5842,42 +5798,42 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5886,12 +5842,12 @@
         <v>-52.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5900,12 +5856,12 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5914,12 +5870,12 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5928,12 +5884,12 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -5942,7 +5898,7 @@
         <v>-20.7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -5956,7 +5912,7 @@
         <v>-52.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -5970,7 +5926,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -5984,7 +5940,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -5998,7 +5954,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Bug fixes for OpenMKM CTI writer
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C80BA7-DAD5-401B-B531-02A650CBF8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDDCBBD-357E-4272-A1C8-DE05BB960569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="123">
   <si>
     <t>name</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>N(S) + H(S) + RU(B) = N-H = NH(S)  + RU(S)</t>
+  </si>
+  <si>
+    <t>n_sites</t>
+  </si>
+  <si>
+    <t>Number of sites occupied by species. Leave blank for gas species. 1 for monodentate species.</t>
   </si>
 </sst>
 </file>
@@ -1279,22 +1285,22 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1386,7 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1425,7 +1431,7 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>2744</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1572,7 +1578,7 @@
       <c r="G7" s="3"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1581,7 +1587,7 @@
       <c r="G8" s="3"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1590,7 +1596,7 @@
       <c r="G9" s="3"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1599,7 +1605,7 @@
       <c r="G10" s="3"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1608,7 +1614,7 @@
       <c r="G11" s="3"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1617,7 +1623,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1626,7 +1632,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1635,7 +1641,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1644,7 +1650,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1653,7 +1659,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1662,7 +1668,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1671,7 +1677,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1680,7 +1686,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1689,7 +1695,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1698,7 +1704,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1707,7 +1713,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1716,7 +1722,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1725,7 +1731,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1734,7 +1740,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1743,7 +1749,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1752,7 +1758,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1761,7 +1767,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1777,28 +1783,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR63"/>
+  <dimension ref="A1:BS63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1815,19 +1821,19 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>51</v>
@@ -1862,10 +1868,12 @@
       <c r="U1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="1"/>
+      <c r="V1" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="Y1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -1910,8 +1918,9 @@
       <c r="BP1" s="1"/>
       <c r="BQ1" s="1"/>
       <c r="BR1" s="1"/>
-    </row>
-    <row r="2" spans="1:70" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BS1" s="1"/>
+    </row>
+    <row r="2" spans="1:71" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1927,20 +1936,20 @@
       <c r="E2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>19</v>
@@ -1975,10 +1984,12 @@
       <c r="U2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="1"/>
+      <c r="V2" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Z2" s="1"/>
+      <c r="Y2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
@@ -2023,8 +2034,9 @@
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1"/>
       <c r="BR2" s="1"/>
-    </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS2" s="1"/>
+    </row>
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2034,25 +2046,24 @@
       <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>-16.63</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>2744</v>
       </c>
-      <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="5"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -2060,10 +2071,10 @@
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
-      <c r="V3" s="1"/>
+      <c r="V3" s="5"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Z3" s="1"/>
+      <c r="Y3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -2108,8 +2119,9 @@
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
-    </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS3" s="1"/>
+    </row>
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2122,31 +2134,30 @@
       <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>-19.54</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>3534</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>3464</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>1765</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>1139</v>
       </c>
-      <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -2154,10 +2165,10 @@
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
-      <c r="V4" s="1"/>
+      <c r="V4" s="5"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="Y4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -2202,8 +2213,9 @@
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
       <c r="BR4" s="1"/>
-    </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS4" s="1"/>
+    </row>
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2213,25 +2225,24 @@
       <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>-6.77</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>4342</v>
       </c>
-      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="5"/>
+      <c r="N5" s="4"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -2239,10 +2250,10 @@
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
-      <c r="V5" s="1"/>
+      <c r="V5" s="5"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="Y5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -2287,8 +2298,9 @@
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
       <c r="BR5" s="1"/>
-    </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS5" s="1"/>
+    </row>
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -2298,40 +2310,42 @@
       <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>-17.239999999999952</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>2197.19</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>360.41500000000002</v>
       </c>
-      <c r="L6" s="4">
+      <c r="M6" s="4">
         <v>347.34300000000002</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>335.67399999999998</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <v>62.076000000000001</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <v>32.179400000000001</v>
       </c>
-      <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
-      <c r="V6" s="1"/>
+      <c r="V6" s="4"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Z6" s="1"/>
+      <c r="Y6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
@@ -2376,8 +2390,9 @@
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
       <c r="BR6" s="1"/>
-    </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS6" s="1"/>
+    </row>
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2387,38 +2402,40 @@
       <c r="E7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>-9.339999999999975</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>549.10500000000002</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>538.55999999999995</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <v>504.32299999999998</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>475.80500000000001</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <v>459.08100000000002</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <v>410.01799999999997</v>
       </c>
-      <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="1"/>
-      <c r="AA7" s="1"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -2451,7 +2468,7 @@
       <c r="BE7" s="1"/>
       <c r="BF7" s="1"/>
       <c r="BG7" s="1"/>
-      <c r="BI7" s="1"/>
+      <c r="BH7" s="1"/>
       <c r="BJ7" s="1"/>
       <c r="BK7" s="1"/>
       <c r="BL7" s="1"/>
@@ -2461,8 +2478,9 @@
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
       <c r="BR7" s="1"/>
-    </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS7" s="1"/>
+    </row>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2472,22 +2490,24 @@
       <c r="E8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <v>-4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <v>1003.51</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>625.54999999999995</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <v>616.29</v>
       </c>
-      <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -2496,8 +2516,8 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="1"/>
-      <c r="AJ8" s="1"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="1"/>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1"/>
       <c r="AM8" s="1"/>
@@ -2521,7 +2541,7 @@
       <c r="BE8" s="1"/>
       <c r="BF8" s="1"/>
       <c r="BG8" s="1"/>
-      <c r="BI8" s="1"/>
+      <c r="BH8" s="1"/>
       <c r="BJ8" s="1"/>
       <c r="BK8" s="1"/>
       <c r="BL8" s="1"/>
@@ -2531,8 +2551,9 @@
       <c r="BP8" s="1"/>
       <c r="BQ8" s="1"/>
       <c r="BR8" s="1"/>
-    </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS8" s="1"/>
+    </row>
+    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -2545,50 +2566,52 @@
       <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>-20.42999999999995</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>3491.0891299999998</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>3488.8194899999999</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <v>3364.5232299999998</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>1583.5157099999999</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <v>1582.0703000000001</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <v>1124.22477</v>
       </c>
-      <c r="P9" s="4">
+      <c r="Q9" s="4">
         <v>570.21231</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="R9" s="4">
         <v>567.22147099999995</v>
       </c>
-      <c r="R9" s="4">
+      <c r="S9" s="4">
         <v>333.08962400000001</v>
       </c>
-      <c r="S9" s="4">
+      <c r="T9" s="4">
         <v>122.859345</v>
       </c>
-      <c r="T9" s="4">
+      <c r="U9" s="4">
         <v>83.828554999999994</v>
       </c>
-      <c r="U9" s="4">
+      <c r="V9" s="4">
         <v>70.625114999999994</v>
       </c>
-      <c r="V9" s="1"/>
-      <c r="AJ9" s="1"/>
+      <c r="W9" s="1"/>
       <c r="AK9" s="1"/>
       <c r="AL9" s="1"/>
       <c r="AM9" s="1"/>
@@ -2612,7 +2635,7 @@
       <c r="BE9" s="1"/>
       <c r="BF9" s="1"/>
       <c r="BG9" s="1"/>
-      <c r="BI9" s="1"/>
+      <c r="BH9" s="1"/>
       <c r="BJ9" s="1"/>
       <c r="BK9" s="1"/>
       <c r="BL9" s="1"/>
@@ -2622,8 +2645,9 @@
       <c r="BP9" s="1"/>
       <c r="BQ9" s="1"/>
       <c r="BR9" s="1"/>
-    </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS9" s="1"/>
+    </row>
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -2636,44 +2660,46 @@
       <c r="E10" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>-16.589999999999975</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>3469.3003399999998</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>3381.05197</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <v>1503.01629</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>698.86880399999995</v>
       </c>
-      <c r="N10" s="4">
+      <c r="O10" s="4">
         <v>625.59609399999999</v>
       </c>
-      <c r="O10" s="4">
+      <c r="P10" s="4">
         <v>615.93978300000003</v>
       </c>
-      <c r="P10" s="4">
+      <c r="Q10" s="4">
         <v>475.130224</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="R10" s="4">
         <v>298.12000999999998</v>
       </c>
-      <c r="R10" s="4">
+      <c r="S10" s="4">
         <v>153.25013899999999</v>
       </c>
-      <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
-      <c r="V10" s="1"/>
-      <c r="AJ10" s="1"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="1"/>
       <c r="AK10" s="1"/>
       <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
@@ -2697,7 +2723,7 @@
       <c r="BE10" s="1"/>
       <c r="BF10" s="1"/>
       <c r="BG10" s="1"/>
-      <c r="BI10" s="1"/>
+      <c r="BH10" s="1"/>
       <c r="BJ10" s="1"/>
       <c r="BK10" s="1"/>
       <c r="BL10" s="1"/>
@@ -2707,8 +2733,9 @@
       <c r="BP10" s="1"/>
       <c r="BQ10" s="1"/>
       <c r="BR10" s="1"/>
-    </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS10" s="1"/>
+    </row>
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -2721,38 +2748,40 @@
       <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>-13.20999999999998</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>3403.12878</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="4">
         <v>718.17758800000001</v>
       </c>
-      <c r="L11" s="4">
+      <c r="M11" s="4">
         <v>710.58051999999998</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>528.52565900000002</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <v>415.19586900000002</v>
       </c>
-      <c r="O11" s="4">
+      <c r="P11" s="4">
         <v>410.13079699999997</v>
       </c>
-      <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-      <c r="V11" s="1"/>
-      <c r="AJ11" s="1"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="1"/>
       <c r="AK11" s="1"/>
       <c r="AL11" s="1"/>
       <c r="AM11" s="1"/>
@@ -2776,7 +2805,7 @@
       <c r="BE11" s="1"/>
       <c r="BF11" s="1"/>
       <c r="BG11" s="1"/>
-      <c r="BI11" s="1"/>
+      <c r="BH11" s="1"/>
       <c r="BJ11" s="1"/>
       <c r="BK11" s="1"/>
       <c r="BL11" s="1"/>
@@ -2786,8 +2815,9 @@
       <c r="BP11" s="1"/>
       <c r="BQ11" s="1"/>
       <c r="BR11" s="1"/>
-    </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS11" s="1"/>
+    </row>
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -2797,49 +2827,51 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="4">
-        <f>I9+1.19</f>
+      <c r="J12" s="4">
+        <f>J9+1.19</f>
         <v>-19.239999999999949</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <v>3453.4106299999999</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="4">
         <v>3355.6699199999998</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="4">
         <v>1723.84977</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <v>1487.9548400000001</v>
       </c>
-      <c r="N12" s="4">
+      <c r="O12" s="4">
         <v>959.15072299999997</v>
       </c>
-      <c r="O12" s="4">
+      <c r="P12" s="4">
         <v>888.94619799999998</v>
       </c>
-      <c r="P12" s="4">
+      <c r="Q12" s="4">
         <v>594.08943899999997</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="R12" s="4">
         <v>428.43113599999998</v>
       </c>
-      <c r="R12" s="4">
+      <c r="S12" s="4">
         <v>227.032386</v>
       </c>
-      <c r="S12" s="4">
+      <c r="T12" s="4">
         <v>206.046727</v>
       </c>
-      <c r="T12" s="4">
+      <c r="U12" s="4">
         <v>142.13585599999999</v>
       </c>
-      <c r="U12" s="4"/>
-      <c r="V12" s="1"/>
-      <c r="AJ12" s="1"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="1"/>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
       <c r="AM12" s="1"/>
@@ -2863,7 +2895,7 @@
       <c r="BE12" s="1"/>
       <c r="BF12" s="1"/>
       <c r="BG12" s="1"/>
-      <c r="BI12" s="1"/>
+      <c r="BH12" s="1"/>
       <c r="BJ12" s="1"/>
       <c r="BK12" s="1"/>
       <c r="BL12" s="1"/>
@@ -2873,8 +2905,9 @@
       <c r="BP12" s="1"/>
       <c r="BQ12" s="1"/>
       <c r="BR12" s="1"/>
-    </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS12" s="1"/>
+    </row>
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -2884,43 +2917,45 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="4">
-        <f>I10+0.72</f>
+      <c r="J13" s="4">
+        <f>J10+0.72</f>
         <v>-15.869999999999974</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <v>3426.4448400000001</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="4">
         <v>1293.72327</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="4">
         <v>922.83076800000003</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <v>660.96659799999998</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="4">
         <v>525.59512400000006</v>
       </c>
-      <c r="O13" s="4">
+      <c r="P13" s="4">
         <v>496.83726300000001</v>
       </c>
-      <c r="P13" s="4">
+      <c r="Q13" s="4">
         <v>330.67445900000001</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="R13" s="4">
         <v>290.27800500000001</v>
       </c>
-      <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
-      <c r="V13" s="1"/>
-      <c r="AJ13" s="1"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="1"/>
       <c r="AK13" s="1"/>
       <c r="AL13" s="1"/>
       <c r="AM13" s="1"/>
@@ -2944,7 +2979,7 @@
       <c r="BE13" s="1"/>
       <c r="BF13" s="1"/>
       <c r="BG13" s="1"/>
-      <c r="BI13" s="1"/>
+      <c r="BH13" s="1"/>
       <c r="BJ13" s="1"/>
       <c r="BK13" s="1"/>
       <c r="BL13" s="1"/>
@@ -2954,8 +2989,9 @@
       <c r="BP13" s="1"/>
       <c r="BQ13" s="1"/>
       <c r="BR13" s="1"/>
-    </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS13" s="1"/>
+    </row>
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -2965,37 +3001,39 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="4">
-        <f>I11+1.28</f>
+      <c r="J14" s="4">
+        <f>J11+1.28</f>
         <v>-11.92999999999998</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>1201.6048699999999</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>491.566416</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="4">
         <v>462.01550200000003</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>402.15890400000001</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <v>242.13872599999999</v>
       </c>
-      <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
-      <c r="V14" s="1"/>
-      <c r="AJ14" s="1"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="1"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
       <c r="AM14" s="1"/>
@@ -3019,7 +3057,7 @@
       <c r="BE14" s="1"/>
       <c r="BF14" s="1"/>
       <c r="BG14" s="1"/>
-      <c r="BI14" s="1"/>
+      <c r="BH14" s="1"/>
       <c r="BJ14" s="1"/>
       <c r="BK14" s="1"/>
       <c r="BL14" s="1"/>
@@ -3029,45 +3067,48 @@
       <c r="BP14" s="1"/>
       <c r="BQ14" s="1"/>
       <c r="BR14" s="1"/>
-    </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS14" s="1"/>
+    </row>
+    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>109</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="4">
-        <f>I6+2.57</f>
+      <c r="J15" s="4">
+        <f>J6+2.57</f>
         <v>-14.669999999999952</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>485.61399999999998</v>
       </c>
-      <c r="K15" s="4">
+      <c r="L15" s="4">
         <v>392.97699999999998</v>
       </c>
-      <c r="L15" s="4">
+      <c r="M15" s="4">
         <v>386.18599999999998</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <v>280.94299999999998</v>
       </c>
-      <c r="N15" s="4">
+      <c r="O15" s="4">
         <v>168.43100000000001</v>
       </c>
-      <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
-      <c r="V15" s="1"/>
-      <c r="AI15" s="1"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
@@ -3091,7 +3132,7 @@
       <c r="BD15" s="1"/>
       <c r="BE15" s="1"/>
       <c r="BF15" s="1"/>
-      <c r="BH15" s="1"/>
+      <c r="BG15" s="1"/>
       <c r="BI15" s="1"/>
       <c r="BJ15" s="1"/>
       <c r="BK15" s="1"/>
@@ -3101,8 +3142,9 @@
       <c r="BO15" s="1"/>
       <c r="BP15" s="1"/>
       <c r="BQ15" s="1"/>
-    </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BR15" s="1"/>
+    </row>
+    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -3112,10 +3154,12 @@
       <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -3128,8 +3172,8 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-      <c r="V16" s="1"/>
-      <c r="AJ16" s="1"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="1"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
@@ -3153,7 +3197,7 @@
       <c r="BE16" s="1"/>
       <c r="BF16" s="1"/>
       <c r="BG16" s="1"/>
-      <c r="BI16" s="1"/>
+      <c r="BH16" s="1"/>
       <c r="BJ16" s="1"/>
       <c r="BK16" s="1"/>
       <c r="BL16" s="1"/>
@@ -3163,8 +3207,9 @@
       <c r="BP16" s="1"/>
       <c r="BQ16" s="1"/>
       <c r="BR16" s="1"/>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS16" s="1"/>
+    </row>
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3174,38 +3219,40 @@
       <c r="E17" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4">
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
         <v>-17.389999999999986</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>1015.734101</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <v>456.07363700000002</v>
       </c>
-      <c r="L17" s="4">
+      <c r="M17" s="4">
         <v>408.12729300000001</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>378.51690000000002</v>
       </c>
-      <c r="N17" s="4">
+      <c r="O17" s="4">
         <v>344.87134400000002</v>
       </c>
-      <c r="O17" s="4">
+      <c r="P17" s="4">
         <v>334.62168200000002</v>
       </c>
-      <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
-      <c r="AJ17" s="1"/>
+      <c r="V17" s="4"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
       <c r="AM17" s="1"/>
@@ -3229,7 +3276,7 @@
       <c r="BE17" s="1"/>
       <c r="BF17" s="1"/>
       <c r="BG17" s="1"/>
-      <c r="BI17" s="1"/>
+      <c r="BH17" s="1"/>
       <c r="BJ17" s="1"/>
       <c r="BK17" s="1"/>
       <c r="BL17" s="1"/>
@@ -3239,8 +3286,9 @@
       <c r="BP17" s="1"/>
       <c r="BQ17" s="1"/>
       <c r="BR17" s="1"/>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS17" s="1"/>
+    </row>
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3250,23 +3298,25 @@
       <c r="E18" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4">
         <v>-9.3899999999999864</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <v>529.80737599999998</v>
       </c>
-      <c r="K18" s="4">
+      <c r="L18" s="4">
         <v>506.95443399999999</v>
       </c>
-      <c r="L18" s="4">
+      <c r="M18" s="4">
         <v>471.09772600000002</v>
       </c>
-      <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -3275,7 +3325,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
-      <c r="AJ18" s="1"/>
+      <c r="V18" s="4"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
@@ -3299,7 +3349,7 @@
       <c r="BE18" s="1"/>
       <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
-      <c r="BI18" s="1"/>
+      <c r="BH18" s="1"/>
       <c r="BJ18" s="1"/>
       <c r="BK18" s="1"/>
       <c r="BL18" s="1"/>
@@ -3309,8 +3359,9 @@
       <c r="BP18" s="1"/>
       <c r="BQ18" s="1"/>
       <c r="BR18" s="1"/>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS18" s="1"/>
+    </row>
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -3320,23 +3371,25 @@
       <c r="E19" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4">
+      <c r="I19" s="4"/>
+      <c r="J19" s="4">
         <v>-4</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <v>1003.51</v>
       </c>
-      <c r="K19" s="4">
+      <c r="L19" s="4">
         <v>625.54999999999995</v>
       </c>
-      <c r="L19" s="4">
+      <c r="M19" s="4">
         <v>616.29</v>
       </c>
-      <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -3345,7 +3398,7 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
-      <c r="AJ19" s="1"/>
+      <c r="V19" s="4"/>
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
       <c r="AM19" s="1"/>
@@ -3369,7 +3422,7 @@
       <c r="BE19" s="1"/>
       <c r="BF19" s="1"/>
       <c r="BG19" s="1"/>
-      <c r="BI19" s="1"/>
+      <c r="BH19" s="1"/>
       <c r="BJ19" s="1"/>
       <c r="BK19" s="1"/>
       <c r="BL19" s="1"/>
@@ -3379,8 +3432,9 @@
       <c r="BP19" s="1"/>
       <c r="BQ19" s="1"/>
       <c r="BR19" s="1"/>
-    </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS19" s="1"/>
+    </row>
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3393,50 +3447,52 @@
       <c r="E20" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4">
+      <c r="I20" s="4"/>
+      <c r="J20" s="4">
         <v>-20.67999999999995</v>
       </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
         <v>3498.0269910000002</v>
       </c>
-      <c r="K20" s="4">
+      <c r="L20" s="4">
         <v>3469.3304969999999</v>
       </c>
-      <c r="L20" s="4">
+      <c r="M20" s="4">
         <v>3362.813486</v>
       </c>
-      <c r="M20" s="4">
+      <c r="N20" s="4">
         <v>1590.9105280000001</v>
       </c>
-      <c r="N20" s="4">
+      <c r="O20" s="4">
         <v>1579.266171</v>
       </c>
-      <c r="O20" s="4">
+      <c r="P20" s="4">
         <v>1140.7628299999999</v>
       </c>
-      <c r="P20" s="4">
+      <c r="Q20" s="4">
         <v>564.97479799999996</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="R20" s="4">
         <v>555.49956799999995</v>
       </c>
-      <c r="R20" s="4">
+      <c r="S20" s="4">
         <v>336.10022600000002</v>
       </c>
-      <c r="S20" s="4">
+      <c r="T20" s="4">
         <v>117.161717</v>
       </c>
-      <c r="T20" s="4">
+      <c r="U20" s="4">
         <v>86.774373999999995</v>
       </c>
-      <c r="U20" s="4">
+      <c r="V20" s="4">
         <v>78.100128999999995</v>
       </c>
-      <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="1"/>
       <c r="AM20" s="1"/>
@@ -3460,7 +3516,7 @@
       <c r="BE20" s="1"/>
       <c r="BF20" s="1"/>
       <c r="BG20" s="1"/>
-      <c r="BI20" s="1"/>
+      <c r="BH20" s="1"/>
       <c r="BJ20" s="1"/>
       <c r="BK20" s="1"/>
       <c r="BL20" s="1"/>
@@ -3470,8 +3526,9 @@
       <c r="BP20" s="1"/>
       <c r="BQ20" s="1"/>
       <c r="BR20" s="1"/>
-    </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS20" s="1"/>
+    </row>
+    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -3484,44 +3541,46 @@
       <c r="E21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4">
+      <c r="I21" s="4"/>
+      <c r="J21" s="4">
         <v>-17.149999999999977</v>
       </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
         <v>3528.6824689999999</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="4">
         <v>3375.447388</v>
       </c>
-      <c r="L21" s="4">
+      <c r="M21" s="4">
         <v>1477.164</v>
       </c>
-      <c r="M21" s="4">
+      <c r="N21" s="4">
         <v>720.07573000000002</v>
       </c>
-      <c r="N21" s="4">
+      <c r="O21" s="4">
         <v>615.66630499999997</v>
       </c>
-      <c r="O21" s="4">
+      <c r="P21" s="4">
         <v>581.96669099999997</v>
       </c>
-      <c r="P21" s="4">
+      <c r="Q21" s="4">
         <v>468.85326900000001</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="R21" s="4">
         <v>286.369823</v>
       </c>
-      <c r="R21" s="4">
+      <c r="S21" s="4">
         <v>105.95658400000001</v>
       </c>
-      <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
-      <c r="AJ21" s="1"/>
+      <c r="V21" s="4"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
       <c r="AM21" s="1"/>
@@ -3545,7 +3604,7 @@
       <c r="BE21" s="1"/>
       <c r="BF21" s="1"/>
       <c r="BG21" s="1"/>
-      <c r="BI21" s="1"/>
+      <c r="BH21" s="1"/>
       <c r="BJ21" s="1"/>
       <c r="BK21" s="1"/>
       <c r="BL21" s="1"/>
@@ -3555,8 +3614,9 @@
       <c r="BP21" s="1"/>
       <c r="BQ21" s="1"/>
       <c r="BR21" s="1"/>
-    </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS21" s="1"/>
+    </row>
+    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -3569,38 +3629,40 @@
       <c r="E22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4">
         <v>-13.1099999999999</v>
       </c>
-      <c r="J22" s="4">
+      <c r="K22" s="4">
         <v>3384.3746510000001</v>
       </c>
-      <c r="K22" s="4">
+      <c r="L22" s="4">
         <v>726.230954</v>
       </c>
-      <c r="L22" s="4">
+      <c r="M22" s="4">
         <v>669.42910800000004</v>
       </c>
-      <c r="M22" s="4">
+      <c r="N22" s="4">
         <v>506.27813500000002</v>
       </c>
-      <c r="N22" s="4">
+      <c r="O22" s="4">
         <v>409.50201399999997</v>
       </c>
-      <c r="O22" s="4">
+      <c r="P22" s="4">
         <v>387.80818099999999</v>
       </c>
-      <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
-      <c r="AJ22" s="1"/>
+      <c r="V22" s="4"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
@@ -3624,7 +3686,7 @@
       <c r="BE22" s="1"/>
       <c r="BF22" s="1"/>
       <c r="BG22" s="1"/>
-      <c r="BI22" s="1"/>
+      <c r="BH22" s="1"/>
       <c r="BJ22" s="1"/>
       <c r="BK22" s="1"/>
       <c r="BL22" s="1"/>
@@ -3634,8 +3696,9 @@
       <c r="BP22" s="1"/>
       <c r="BQ22" s="1"/>
       <c r="BR22" s="1"/>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS22" s="1"/>
+    </row>
+    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3646,48 +3709,50 @@
         <v>3</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" t="s">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4">
+      <c r="I23" s="4"/>
+      <c r="J23" s="4">
         <v>-19.809999999999945</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <v>3484.3961949999998</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="4">
         <v>3385.2659090000002</v>
       </c>
-      <c r="L23" s="4">
+      <c r="M23" s="4">
         <v>1685.8293080000001</v>
       </c>
-      <c r="M23" s="4">
+      <c r="N23" s="4">
         <v>1480.998257</v>
       </c>
-      <c r="N23" s="4">
+      <c r="O23" s="4">
         <v>1002.067555</v>
       </c>
-      <c r="O23" s="4">
+      <c r="P23" s="4">
         <v>916.14745100000005</v>
       </c>
-      <c r="P23" s="4">
+      <c r="Q23" s="4">
         <v>575.40527899999995</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="R23" s="4">
         <v>431.30664400000001</v>
       </c>
-      <c r="R23" s="4">
+      <c r="S23" s="4">
         <v>345.148708</v>
       </c>
-      <c r="S23" s="4">
+      <c r="T23" s="4">
         <v>221.64965799999999</v>
       </c>
-      <c r="T23" s="4">
+      <c r="U23" s="4">
         <v>70.339661000000007</v>
       </c>
-      <c r="U23" s="4"/>
-      <c r="AJ23" s="1"/>
+      <c r="V23" s="4"/>
       <c r="AK23" s="1"/>
       <c r="AL23" s="1"/>
       <c r="AM23" s="1"/>
@@ -3711,7 +3776,7 @@
       <c r="BE23" s="1"/>
       <c r="BF23" s="1"/>
       <c r="BG23" s="1"/>
-      <c r="BI23" s="1"/>
+      <c r="BH23" s="1"/>
       <c r="BJ23" s="1"/>
       <c r="BK23" s="1"/>
       <c r="BL23" s="1"/>
@@ -3721,8 +3786,9 @@
       <c r="BP23" s="1"/>
       <c r="BQ23" s="1"/>
       <c r="BR23" s="1"/>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS23" s="1"/>
+    </row>
+    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3733,42 +3799,44 @@
         <v>2</v>
       </c>
       <c r="E24" s="10"/>
-      <c r="F24" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4">
+      <c r="I24" s="4"/>
+      <c r="J24" s="4">
         <v>-15.819999999999936</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <v>3432.815967</v>
       </c>
-      <c r="K24" s="4">
+      <c r="L24" s="4">
         <v>1789.8865699999999</v>
       </c>
-      <c r="L24" s="4">
+      <c r="M24" s="4">
         <v>1032.1897269999999</v>
       </c>
-      <c r="M24" s="4">
+      <c r="N24" s="4">
         <v>583.47939799999995</v>
       </c>
-      <c r="N24" s="4">
+      <c r="O24" s="4">
         <v>392.83707299999998</v>
       </c>
-      <c r="O24" s="4">
+      <c r="P24" s="4">
         <v>384.833597</v>
       </c>
-      <c r="P24" s="4">
+      <c r="Q24" s="4">
         <v>311.60087600000003</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="R24" s="4">
         <v>110.96862400000001</v>
       </c>
-      <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
-      <c r="AJ24" s="1"/>
+      <c r="V24" s="4"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
@@ -3792,7 +3860,7 @@
       <c r="BE24" s="1"/>
       <c r="BF24" s="1"/>
       <c r="BG24" s="1"/>
-      <c r="BI24" s="1"/>
+      <c r="BH24" s="1"/>
       <c r="BJ24" s="1"/>
       <c r="BK24" s="1"/>
       <c r="BL24" s="1"/>
@@ -3802,8 +3870,9 @@
       <c r="BP24" s="1"/>
       <c r="BQ24" s="1"/>
       <c r="BR24" s="1"/>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS24" s="1"/>
+    </row>
+    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -3814,36 +3883,38 @@
         <v>1</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" t="s">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4">
+      <c r="I25" s="4"/>
+      <c r="J25" s="4">
         <v>-12.120000000000005</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>1679.786106</v>
       </c>
-      <c r="K25" s="4">
+      <c r="L25" s="4">
         <v>509.64356400000003</v>
       </c>
-      <c r="L25" s="4">
+      <c r="M25" s="4">
         <v>489.064573</v>
       </c>
-      <c r="M25" s="4">
+      <c r="N25" s="4">
         <v>443.45080000000002</v>
       </c>
-      <c r="N25" s="4">
+      <c r="O25" s="4">
         <v>396.19289099999997</v>
       </c>
-      <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
-      <c r="AJ25" s="1"/>
+      <c r="V25" s="4"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
       <c r="AM25" s="1"/>
@@ -3867,7 +3938,7 @@
       <c r="BE25" s="1"/>
       <c r="BF25" s="1"/>
       <c r="BG25" s="1"/>
-      <c r="BI25" s="1"/>
+      <c r="BH25" s="1"/>
       <c r="BJ25" s="1"/>
       <c r="BK25" s="1"/>
       <c r="BL25" s="1"/>
@@ -3877,8 +3948,9 @@
       <c r="BP25" s="1"/>
       <c r="BQ25" s="1"/>
       <c r="BR25" s="1"/>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS25" s="1"/>
+    </row>
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3886,36 +3958,38 @@
         <v>2</v>
       </c>
       <c r="E26" s="10"/>
-      <c r="F26" t="s">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4">
+      <c r="I26" s="4"/>
+      <c r="J26" s="4">
         <v>-16.799999999999955</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>549.17255799999998</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>496.630066</v>
       </c>
-      <c r="L26" s="4">
+      <c r="M26" s="4">
         <v>436.16551199999998</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>418.36746199999999</v>
       </c>
-      <c r="N26" s="4">
+      <c r="O26" s="4">
         <v>391.94338199999999</v>
       </c>
-      <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
-      <c r="AJ26" s="1"/>
+      <c r="V26" s="4"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
       <c r="AM26" s="1"/>
@@ -3939,7 +4013,7 @@
       <c r="BE26" s="1"/>
       <c r="BF26" s="1"/>
       <c r="BG26" s="1"/>
-      <c r="BI26" s="1"/>
+      <c r="BH26" s="1"/>
       <c r="BJ26" s="1"/>
       <c r="BK26" s="1"/>
       <c r="BL26" s="1"/>
@@ -3949,8 +4023,9 @@
       <c r="BP26" s="1"/>
       <c r="BQ26" s="1"/>
       <c r="BR26" s="1"/>
-    </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS26" s="1"/>
+    </row>
+    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -3960,10 +4035,12 @@
       <c r="E27" t="s">
         <v>111</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -3976,8 +4053,8 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
-      <c r="V27" s="1"/>
-      <c r="AJ27" s="1"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
       <c r="AM27" s="1"/>
@@ -4001,7 +4078,7 @@
       <c r="BE27" s="1"/>
       <c r="BF27" s="1"/>
       <c r="BG27" s="1"/>
-      <c r="BI27" s="1"/>
+      <c r="BH27" s="1"/>
       <c r="BJ27" s="1"/>
       <c r="BK27" s="1"/>
       <c r="BL27" s="1"/>
@@ -4011,8 +4088,9 @@
       <c r="BP27" s="1"/>
       <c r="BQ27" s="1"/>
       <c r="BR27" s="1"/>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS27" s="1"/>
+    </row>
+    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4022,10 +4100,12 @@
       <c r="E28" t="s">
         <v>54</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -4038,8 +4118,8 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
-      <c r="V28" s="1"/>
-      <c r="AJ28" s="1"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="1"/>
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
       <c r="AM28" s="1"/>
@@ -4063,7 +4143,7 @@
       <c r="BE28" s="1"/>
       <c r="BF28" s="1"/>
       <c r="BG28" s="1"/>
-      <c r="BI28" s="1"/>
+      <c r="BH28" s="1"/>
       <c r="BJ28" s="1"/>
       <c r="BK28" s="1"/>
       <c r="BL28" s="1"/>
@@ -4073,10 +4153,11 @@
       <c r="BP28" s="1"/>
       <c r="BQ28" s="1"/>
       <c r="BR28" s="1"/>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS28" s="1"/>
+    </row>
+    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
-      <c r="AJ29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="AK29" s="1"/>
       <c r="AL29" s="1"/>
       <c r="AM29" s="1"/>
@@ -4100,7 +4181,7 @@
       <c r="BE29" s="1"/>
       <c r="BF29" s="1"/>
       <c r="BG29" s="1"/>
-      <c r="BI29" s="1"/>
+      <c r="BH29" s="1"/>
       <c r="BJ29" s="1"/>
       <c r="BK29" s="1"/>
       <c r="BL29" s="1"/>
@@ -4110,10 +4191,11 @@
       <c r="BP29" s="1"/>
       <c r="BQ29" s="1"/>
       <c r="BR29" s="1"/>
-    </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS29" s="1"/>
+    </row>
+    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
-      <c r="AJ30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
       <c r="AM30" s="1"/>
@@ -4137,7 +4219,7 @@
       <c r="BE30" s="1"/>
       <c r="BF30" s="1"/>
       <c r="BG30" s="1"/>
-      <c r="BI30" s="1"/>
+      <c r="BH30" s="1"/>
       <c r="BJ30" s="1"/>
       <c r="BK30" s="1"/>
       <c r="BL30" s="1"/>
@@ -4147,10 +4229,11 @@
       <c r="BP30" s="1"/>
       <c r="BQ30" s="1"/>
       <c r="BR30" s="1"/>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS30" s="1"/>
+    </row>
+    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
-      <c r="AJ31" s="1"/>
+      <c r="F31" s="1"/>
       <c r="AK31" s="1"/>
       <c r="AL31" s="1"/>
       <c r="AM31" s="1"/>
@@ -4174,7 +4257,7 @@
       <c r="BE31" s="1"/>
       <c r="BF31" s="1"/>
       <c r="BG31" s="1"/>
-      <c r="BI31" s="1"/>
+      <c r="BH31" s="1"/>
       <c r="BJ31" s="1"/>
       <c r="BK31" s="1"/>
       <c r="BL31" s="1"/>
@@ -4184,10 +4267,11 @@
       <c r="BP31" s="1"/>
       <c r="BQ31" s="1"/>
       <c r="BR31" s="1"/>
-    </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BS31" s="1"/>
+    </row>
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
-      <c r="AJ32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
       <c r="AM32" s="1"/>
@@ -4211,7 +4295,7 @@
       <c r="BE32" s="1"/>
       <c r="BF32" s="1"/>
       <c r="BG32" s="1"/>
-      <c r="BI32" s="1"/>
+      <c r="BH32" s="1"/>
       <c r="BJ32" s="1"/>
       <c r="BK32" s="1"/>
       <c r="BL32" s="1"/>
@@ -4221,10 +4305,11 @@
       <c r="BP32" s="1"/>
       <c r="BQ32" s="1"/>
       <c r="BR32" s="1"/>
-    </row>
-    <row r="33" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS32" s="1"/>
+    </row>
+    <row r="33" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
-      <c r="AJ33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
       <c r="AM33" s="1"/>
@@ -4248,7 +4333,7 @@
       <c r="BE33" s="1"/>
       <c r="BF33" s="1"/>
       <c r="BG33" s="1"/>
-      <c r="BI33" s="1"/>
+      <c r="BH33" s="1"/>
       <c r="BJ33" s="1"/>
       <c r="BK33" s="1"/>
       <c r="BL33" s="1"/>
@@ -4258,10 +4343,11 @@
       <c r="BP33" s="1"/>
       <c r="BQ33" s="1"/>
       <c r="BR33" s="1"/>
-    </row>
-    <row r="34" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS33" s="1"/>
+    </row>
+    <row r="34" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
-      <c r="AJ34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
       <c r="AM34" s="1"/>
@@ -4285,7 +4371,7 @@
       <c r="BE34" s="1"/>
       <c r="BF34" s="1"/>
       <c r="BG34" s="1"/>
-      <c r="BI34" s="1"/>
+      <c r="BH34" s="1"/>
       <c r="BJ34" s="1"/>
       <c r="BK34" s="1"/>
       <c r="BL34" s="1"/>
@@ -4295,10 +4381,11 @@
       <c r="BP34" s="1"/>
       <c r="BQ34" s="1"/>
       <c r="BR34" s="1"/>
-    </row>
-    <row r="35" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS34" s="1"/>
+    </row>
+    <row r="35" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
-      <c r="AJ35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="AK35" s="1"/>
       <c r="AL35" s="1"/>
       <c r="AM35" s="1"/>
@@ -4322,7 +4409,7 @@
       <c r="BE35" s="1"/>
       <c r="BF35" s="1"/>
       <c r="BG35" s="1"/>
-      <c r="BI35" s="1"/>
+      <c r="BH35" s="1"/>
       <c r="BJ35" s="1"/>
       <c r="BK35" s="1"/>
       <c r="BL35" s="1"/>
@@ -4332,10 +4419,11 @@
       <c r="BP35" s="1"/>
       <c r="BQ35" s="1"/>
       <c r="BR35" s="1"/>
-    </row>
-    <row r="36" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS35" s="1"/>
+    </row>
+    <row r="36" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
-      <c r="AJ36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="AK36" s="1"/>
       <c r="AL36" s="1"/>
       <c r="AM36" s="1"/>
@@ -4359,7 +4447,7 @@
       <c r="BE36" s="1"/>
       <c r="BF36" s="1"/>
       <c r="BG36" s="1"/>
-      <c r="BI36" s="1"/>
+      <c r="BH36" s="1"/>
       <c r="BJ36" s="1"/>
       <c r="BK36" s="1"/>
       <c r="BL36" s="1"/>
@@ -4369,10 +4457,11 @@
       <c r="BP36" s="1"/>
       <c r="BQ36" s="1"/>
       <c r="BR36" s="1"/>
-    </row>
-    <row r="37" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS36" s="1"/>
+    </row>
+    <row r="37" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
-      <c r="AJ37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="AK37" s="1"/>
       <c r="AL37" s="1"/>
       <c r="AM37" s="1"/>
@@ -4396,7 +4485,7 @@
       <c r="BE37" s="1"/>
       <c r="BF37" s="1"/>
       <c r="BG37" s="1"/>
-      <c r="BI37" s="1"/>
+      <c r="BH37" s="1"/>
       <c r="BJ37" s="1"/>
       <c r="BK37" s="1"/>
       <c r="BL37" s="1"/>
@@ -4406,10 +4495,11 @@
       <c r="BP37" s="1"/>
       <c r="BQ37" s="1"/>
       <c r="BR37" s="1"/>
-    </row>
-    <row r="38" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS37" s="1"/>
+    </row>
+    <row r="38" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
-      <c r="AJ38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="AK38" s="1"/>
       <c r="AL38" s="1"/>
       <c r="AM38" s="1"/>
@@ -4433,7 +4523,7 @@
       <c r="BE38" s="1"/>
       <c r="BF38" s="1"/>
       <c r="BG38" s="1"/>
-      <c r="BI38" s="1"/>
+      <c r="BH38" s="1"/>
       <c r="BJ38" s="1"/>
       <c r="BK38" s="1"/>
       <c r="BL38" s="1"/>
@@ -4443,10 +4533,11 @@
       <c r="BP38" s="1"/>
       <c r="BQ38" s="1"/>
       <c r="BR38" s="1"/>
-    </row>
-    <row r="39" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS38" s="1"/>
+    </row>
+    <row r="39" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
-      <c r="AJ39" s="1"/>
+      <c r="F39" s="1"/>
       <c r="AK39" s="1"/>
       <c r="AL39" s="1"/>
       <c r="AM39" s="1"/>
@@ -4470,7 +4561,7 @@
       <c r="BE39" s="1"/>
       <c r="BF39" s="1"/>
       <c r="BG39" s="1"/>
-      <c r="BI39" s="1"/>
+      <c r="BH39" s="1"/>
       <c r="BJ39" s="1"/>
       <c r="BK39" s="1"/>
       <c r="BL39" s="1"/>
@@ -4480,10 +4571,11 @@
       <c r="BP39" s="1"/>
       <c r="BQ39" s="1"/>
       <c r="BR39" s="1"/>
-    </row>
-    <row r="40" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS39" s="1"/>
+    </row>
+    <row r="40" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
-      <c r="AJ40" s="1"/>
+      <c r="F40" s="1"/>
       <c r="AK40" s="1"/>
       <c r="AL40" s="1"/>
       <c r="AM40" s="1"/>
@@ -4507,7 +4599,7 @@
       <c r="BE40" s="1"/>
       <c r="BF40" s="1"/>
       <c r="BG40" s="1"/>
-      <c r="BI40" s="1"/>
+      <c r="BH40" s="1"/>
       <c r="BJ40" s="1"/>
       <c r="BK40" s="1"/>
       <c r="BL40" s="1"/>
@@ -4517,10 +4609,11 @@
       <c r="BP40" s="1"/>
       <c r="BQ40" s="1"/>
       <c r="BR40" s="1"/>
-    </row>
-    <row r="41" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS40" s="1"/>
+    </row>
+    <row r="41" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
-      <c r="AJ41" s="1"/>
+      <c r="F41" s="1"/>
       <c r="AK41" s="1"/>
       <c r="AL41" s="1"/>
       <c r="AM41" s="1"/>
@@ -4544,7 +4637,7 @@
       <c r="BE41" s="1"/>
       <c r="BF41" s="1"/>
       <c r="BG41" s="1"/>
-      <c r="BI41" s="1"/>
+      <c r="BH41" s="1"/>
       <c r="BJ41" s="1"/>
       <c r="BK41" s="1"/>
       <c r="BL41" s="1"/>
@@ -4554,10 +4647,11 @@
       <c r="BP41" s="1"/>
       <c r="BQ41" s="1"/>
       <c r="BR41" s="1"/>
-    </row>
-    <row r="42" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS41" s="1"/>
+    </row>
+    <row r="42" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E42" s="1"/>
-      <c r="AJ42" s="1"/>
+      <c r="F42" s="1"/>
       <c r="AK42" s="1"/>
       <c r="AL42" s="1"/>
       <c r="AM42" s="1"/>
@@ -4581,7 +4675,7 @@
       <c r="BE42" s="1"/>
       <c r="BF42" s="1"/>
       <c r="BG42" s="1"/>
-      <c r="BI42" s="1"/>
+      <c r="BH42" s="1"/>
       <c r="BJ42" s="1"/>
       <c r="BK42" s="1"/>
       <c r="BL42" s="1"/>
@@ -4591,10 +4685,11 @@
       <c r="BP42" s="1"/>
       <c r="BQ42" s="1"/>
       <c r="BR42" s="1"/>
-    </row>
-    <row r="43" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS42" s="1"/>
+    </row>
+    <row r="43" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E43" s="1"/>
-      <c r="AJ43" s="1"/>
+      <c r="F43" s="1"/>
       <c r="AK43" s="1"/>
       <c r="AL43" s="1"/>
       <c r="AM43" s="1"/>
@@ -4618,7 +4713,7 @@
       <c r="BE43" s="1"/>
       <c r="BF43" s="1"/>
       <c r="BG43" s="1"/>
-      <c r="BI43" s="1"/>
+      <c r="BH43" s="1"/>
       <c r="BJ43" s="1"/>
       <c r="BK43" s="1"/>
       <c r="BL43" s="1"/>
@@ -4628,10 +4723,11 @@
       <c r="BP43" s="1"/>
       <c r="BQ43" s="1"/>
       <c r="BR43" s="1"/>
-    </row>
-    <row r="44" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS43" s="1"/>
+    </row>
+    <row r="44" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E44" s="1"/>
-      <c r="AJ44" s="1"/>
+      <c r="F44" s="1"/>
       <c r="AK44" s="1"/>
       <c r="AL44" s="1"/>
       <c r="AM44" s="1"/>
@@ -4655,7 +4751,7 @@
       <c r="BE44" s="1"/>
       <c r="BF44" s="1"/>
       <c r="BG44" s="1"/>
-      <c r="BI44" s="1"/>
+      <c r="BH44" s="1"/>
       <c r="BJ44" s="1"/>
       <c r="BK44" s="1"/>
       <c r="BL44" s="1"/>
@@ -4665,10 +4761,11 @@
       <c r="BP44" s="1"/>
       <c r="BQ44" s="1"/>
       <c r="BR44" s="1"/>
-    </row>
-    <row r="45" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS44" s="1"/>
+    </row>
+    <row r="45" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
-      <c r="AJ45" s="1"/>
+      <c r="F45" s="1"/>
       <c r="AK45" s="1"/>
       <c r="AL45" s="1"/>
       <c r="AM45" s="1"/>
@@ -4692,7 +4789,7 @@
       <c r="BE45" s="1"/>
       <c r="BF45" s="1"/>
       <c r="BG45" s="1"/>
-      <c r="BI45" s="1"/>
+      <c r="BH45" s="1"/>
       <c r="BJ45" s="1"/>
       <c r="BK45" s="1"/>
       <c r="BL45" s="1"/>
@@ -4702,10 +4799,11 @@
       <c r="BP45" s="1"/>
       <c r="BQ45" s="1"/>
       <c r="BR45" s="1"/>
-    </row>
-    <row r="46" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS45" s="1"/>
+    </row>
+    <row r="46" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E46" s="1"/>
-      <c r="AJ46" s="1"/>
+      <c r="F46" s="1"/>
       <c r="AK46" s="1"/>
       <c r="AL46" s="1"/>
       <c r="AM46" s="1"/>
@@ -4729,7 +4827,7 @@
       <c r="BE46" s="1"/>
       <c r="BF46" s="1"/>
       <c r="BG46" s="1"/>
-      <c r="BI46" s="1"/>
+      <c r="BH46" s="1"/>
       <c r="BJ46" s="1"/>
       <c r="BK46" s="1"/>
       <c r="BL46" s="1"/>
@@ -4739,10 +4837,11 @@
       <c r="BP46" s="1"/>
       <c r="BQ46" s="1"/>
       <c r="BR46" s="1"/>
-    </row>
-    <row r="47" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS46" s="1"/>
+    </row>
+    <row r="47" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E47" s="1"/>
-      <c r="AJ47" s="1"/>
+      <c r="F47" s="1"/>
       <c r="AK47" s="1"/>
       <c r="AL47" s="1"/>
       <c r="AM47" s="1"/>
@@ -4766,7 +4865,7 @@
       <c r="BE47" s="1"/>
       <c r="BF47" s="1"/>
       <c r="BG47" s="1"/>
-      <c r="BI47" s="1"/>
+      <c r="BH47" s="1"/>
       <c r="BJ47" s="1"/>
       <c r="BK47" s="1"/>
       <c r="BL47" s="1"/>
@@ -4776,10 +4875,11 @@
       <c r="BP47" s="1"/>
       <c r="BQ47" s="1"/>
       <c r="BR47" s="1"/>
-    </row>
-    <row r="48" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS47" s="1"/>
+    </row>
+    <row r="48" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E48" s="1"/>
-      <c r="AJ48" s="1"/>
+      <c r="F48" s="1"/>
       <c r="AK48" s="1"/>
       <c r="AL48" s="1"/>
       <c r="AM48" s="1"/>
@@ -4803,7 +4903,7 @@
       <c r="BE48" s="1"/>
       <c r="BF48" s="1"/>
       <c r="BG48" s="1"/>
-      <c r="BI48" s="1"/>
+      <c r="BH48" s="1"/>
       <c r="BJ48" s="1"/>
       <c r="BK48" s="1"/>
       <c r="BL48" s="1"/>
@@ -4813,10 +4913,11 @@
       <c r="BP48" s="1"/>
       <c r="BQ48" s="1"/>
       <c r="BR48" s="1"/>
-    </row>
-    <row r="49" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS48" s="1"/>
+    </row>
+    <row r="49" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E49" s="1"/>
-      <c r="AJ49" s="1"/>
+      <c r="F49" s="1"/>
       <c r="AK49" s="1"/>
       <c r="AL49" s="1"/>
       <c r="AM49" s="1"/>
@@ -4840,7 +4941,7 @@
       <c r="BE49" s="1"/>
       <c r="BF49" s="1"/>
       <c r="BG49" s="1"/>
-      <c r="BI49" s="1"/>
+      <c r="BH49" s="1"/>
       <c r="BJ49" s="1"/>
       <c r="BK49" s="1"/>
       <c r="BL49" s="1"/>
@@ -4850,10 +4951,11 @@
       <c r="BP49" s="1"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
-    </row>
-    <row r="50" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS49" s="1"/>
+    </row>
+    <row r="50" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E50" s="1"/>
-      <c r="AJ50" s="1"/>
+      <c r="F50" s="1"/>
       <c r="AK50" s="1"/>
       <c r="AL50" s="1"/>
       <c r="AM50" s="1"/>
@@ -4877,7 +4979,7 @@
       <c r="BE50" s="1"/>
       <c r="BF50" s="1"/>
       <c r="BG50" s="1"/>
-      <c r="BI50" s="1"/>
+      <c r="BH50" s="1"/>
       <c r="BJ50" s="1"/>
       <c r="BK50" s="1"/>
       <c r="BL50" s="1"/>
@@ -4887,10 +4989,11 @@
       <c r="BP50" s="1"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
-    </row>
-    <row r="51" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS50" s="1"/>
+    </row>
+    <row r="51" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E51" s="1"/>
-      <c r="AJ51" s="1"/>
+      <c r="F51" s="1"/>
       <c r="AK51" s="1"/>
       <c r="AL51" s="1"/>
       <c r="AM51" s="1"/>
@@ -4914,7 +5017,7 @@
       <c r="BE51" s="1"/>
       <c r="BF51" s="1"/>
       <c r="BG51" s="1"/>
-      <c r="BI51" s="1"/>
+      <c r="BH51" s="1"/>
       <c r="BJ51" s="1"/>
       <c r="BK51" s="1"/>
       <c r="BL51" s="1"/>
@@ -4924,10 +5027,11 @@
       <c r="BP51" s="1"/>
       <c r="BQ51" s="1"/>
       <c r="BR51" s="1"/>
-    </row>
-    <row r="52" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS51" s="1"/>
+    </row>
+    <row r="52" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E52" s="1"/>
-      <c r="AJ52" s="1"/>
+      <c r="F52" s="1"/>
       <c r="AK52" s="1"/>
       <c r="AL52" s="1"/>
       <c r="AM52" s="1"/>
@@ -4951,7 +5055,7 @@
       <c r="BE52" s="1"/>
       <c r="BF52" s="1"/>
       <c r="BG52" s="1"/>
-      <c r="BI52" s="1"/>
+      <c r="BH52" s="1"/>
       <c r="BJ52" s="1"/>
       <c r="BK52" s="1"/>
       <c r="BL52" s="1"/>
@@ -4961,10 +5065,11 @@
       <c r="BP52" s="1"/>
       <c r="BQ52" s="1"/>
       <c r="BR52" s="1"/>
-    </row>
-    <row r="53" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS52" s="1"/>
+    </row>
+    <row r="53" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E53" s="1"/>
-      <c r="AJ53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="1"/>
       <c r="AM53" s="1"/>
@@ -4988,7 +5093,7 @@
       <c r="BE53" s="1"/>
       <c r="BF53" s="1"/>
       <c r="BG53" s="1"/>
-      <c r="BI53" s="1"/>
+      <c r="BH53" s="1"/>
       <c r="BJ53" s="1"/>
       <c r="BK53" s="1"/>
       <c r="BL53" s="1"/>
@@ -4998,10 +5103,11 @@
       <c r="BP53" s="1"/>
       <c r="BQ53" s="1"/>
       <c r="BR53" s="1"/>
-    </row>
-    <row r="54" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS53" s="1"/>
+    </row>
+    <row r="54" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E54" s="1"/>
-      <c r="AJ54" s="1"/>
+      <c r="F54" s="1"/>
       <c r="AK54" s="1"/>
       <c r="AL54" s="1"/>
       <c r="AM54" s="1"/>
@@ -5025,7 +5131,7 @@
       <c r="BE54" s="1"/>
       <c r="BF54" s="1"/>
       <c r="BG54" s="1"/>
-      <c r="BI54" s="1"/>
+      <c r="BH54" s="1"/>
       <c r="BJ54" s="1"/>
       <c r="BK54" s="1"/>
       <c r="BL54" s="1"/>
@@ -5035,10 +5141,11 @@
       <c r="BP54" s="1"/>
       <c r="BQ54" s="1"/>
       <c r="BR54" s="1"/>
-    </row>
-    <row r="55" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS54" s="1"/>
+    </row>
+    <row r="55" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
-      <c r="AJ55" s="1"/>
+      <c r="F55" s="1"/>
       <c r="AK55" s="1"/>
       <c r="AL55" s="1"/>
       <c r="AM55" s="1"/>
@@ -5062,7 +5169,7 @@
       <c r="BE55" s="1"/>
       <c r="BF55" s="1"/>
       <c r="BG55" s="1"/>
-      <c r="BI55" s="1"/>
+      <c r="BH55" s="1"/>
       <c r="BJ55" s="1"/>
       <c r="BK55" s="1"/>
       <c r="BL55" s="1"/>
@@ -5072,10 +5179,11 @@
       <c r="BP55" s="1"/>
       <c r="BQ55" s="1"/>
       <c r="BR55" s="1"/>
-    </row>
-    <row r="56" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS55" s="1"/>
+    </row>
+    <row r="56" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
-      <c r="AJ56" s="1"/>
+      <c r="F56" s="1"/>
       <c r="AK56" s="1"/>
       <c r="AL56" s="1"/>
       <c r="AM56" s="1"/>
@@ -5099,7 +5207,7 @@
       <c r="BE56" s="1"/>
       <c r="BF56" s="1"/>
       <c r="BG56" s="1"/>
-      <c r="BI56" s="1"/>
+      <c r="BH56" s="1"/>
       <c r="BJ56" s="1"/>
       <c r="BK56" s="1"/>
       <c r="BL56" s="1"/>
@@ -5109,10 +5217,11 @@
       <c r="BP56" s="1"/>
       <c r="BQ56" s="1"/>
       <c r="BR56" s="1"/>
-    </row>
-    <row r="57" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS56" s="1"/>
+    </row>
+    <row r="57" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
-      <c r="AJ57" s="1"/>
+      <c r="F57" s="1"/>
       <c r="AK57" s="1"/>
       <c r="AL57" s="1"/>
       <c r="AM57" s="1"/>
@@ -5136,7 +5245,7 @@
       <c r="BE57" s="1"/>
       <c r="BF57" s="1"/>
       <c r="BG57" s="1"/>
-      <c r="BI57" s="1"/>
+      <c r="BH57" s="1"/>
       <c r="BJ57" s="1"/>
       <c r="BK57" s="1"/>
       <c r="BL57" s="1"/>
@@ -5146,10 +5255,11 @@
       <c r="BP57" s="1"/>
       <c r="BQ57" s="1"/>
       <c r="BR57" s="1"/>
-    </row>
-    <row r="58" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS57" s="1"/>
+    </row>
+    <row r="58" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
-      <c r="AJ58" s="1"/>
+      <c r="F58" s="1"/>
       <c r="AK58" s="1"/>
       <c r="AL58" s="1"/>
       <c r="AM58" s="1"/>
@@ -5173,7 +5283,7 @@
       <c r="BE58" s="1"/>
       <c r="BF58" s="1"/>
       <c r="BG58" s="1"/>
-      <c r="BI58" s="1"/>
+      <c r="BH58" s="1"/>
       <c r="BJ58" s="1"/>
       <c r="BK58" s="1"/>
       <c r="BL58" s="1"/>
@@ -5183,10 +5293,11 @@
       <c r="BP58" s="1"/>
       <c r="BQ58" s="1"/>
       <c r="BR58" s="1"/>
-    </row>
-    <row r="59" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS58" s="1"/>
+    </row>
+    <row r="59" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
-      <c r="AJ59" s="1"/>
+      <c r="F59" s="1"/>
       <c r="AK59" s="1"/>
       <c r="AL59" s="1"/>
       <c r="AM59" s="1"/>
@@ -5210,7 +5321,7 @@
       <c r="BE59" s="1"/>
       <c r="BF59" s="1"/>
       <c r="BG59" s="1"/>
-      <c r="BI59" s="1"/>
+      <c r="BH59" s="1"/>
       <c r="BJ59" s="1"/>
       <c r="BK59" s="1"/>
       <c r="BL59" s="1"/>
@@ -5220,10 +5331,11 @@
       <c r="BP59" s="1"/>
       <c r="BQ59" s="1"/>
       <c r="BR59" s="1"/>
-    </row>
-    <row r="60" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS59" s="1"/>
+    </row>
+    <row r="60" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
-      <c r="AJ60" s="1"/>
+      <c r="F60" s="1"/>
       <c r="AK60" s="1"/>
       <c r="AL60" s="1"/>
       <c r="AM60" s="1"/>
@@ -5247,7 +5359,7 @@
       <c r="BE60" s="1"/>
       <c r="BF60" s="1"/>
       <c r="BG60" s="1"/>
-      <c r="BI60" s="1"/>
+      <c r="BH60" s="1"/>
       <c r="BJ60" s="1"/>
       <c r="BK60" s="1"/>
       <c r="BL60" s="1"/>
@@ -5257,10 +5369,11 @@
       <c r="BP60" s="1"/>
       <c r="BQ60" s="1"/>
       <c r="BR60" s="1"/>
-    </row>
-    <row r="61" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS60" s="1"/>
+    </row>
+    <row r="61" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
-      <c r="AJ61" s="1"/>
+      <c r="F61" s="1"/>
       <c r="AK61" s="1"/>
       <c r="AL61" s="1"/>
       <c r="AM61" s="1"/>
@@ -5284,7 +5397,7 @@
       <c r="BE61" s="1"/>
       <c r="BF61" s="1"/>
       <c r="BG61" s="1"/>
-      <c r="BI61" s="1"/>
+      <c r="BH61" s="1"/>
       <c r="BJ61" s="1"/>
       <c r="BK61" s="1"/>
       <c r="BL61" s="1"/>
@@ -5294,10 +5407,11 @@
       <c r="BP61" s="1"/>
       <c r="BQ61" s="1"/>
       <c r="BR61" s="1"/>
-    </row>
-    <row r="62" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS61" s="1"/>
+    </row>
+    <row r="62" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E62" s="1"/>
-      <c r="AJ62" s="1"/>
+      <c r="F62" s="1"/>
       <c r="AK62" s="1"/>
       <c r="AL62" s="1"/>
       <c r="AM62" s="1"/>
@@ -5321,7 +5435,7 @@
       <c r="BE62" s="1"/>
       <c r="BF62" s="1"/>
       <c r="BG62" s="1"/>
-      <c r="BI62" s="1"/>
+      <c r="BH62" s="1"/>
       <c r="BJ62" s="1"/>
       <c r="BK62" s="1"/>
       <c r="BL62" s="1"/>
@@ -5331,10 +5445,11 @@
       <c r="BP62" s="1"/>
       <c r="BQ62" s="1"/>
       <c r="BR62" s="1"/>
-    </row>
-    <row r="63" spans="5:70" x14ac:dyDescent="0.3">
+      <c r="BS62" s="1"/>
+    </row>
+    <row r="63" spans="5:71" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
-      <c r="AJ63" s="1"/>
+      <c r="F63" s="1"/>
       <c r="AK63" s="1"/>
       <c r="AL63" s="1"/>
       <c r="AM63" s="1"/>
@@ -5358,7 +5473,7 @@
       <c r="BE63" s="1"/>
       <c r="BF63" s="1"/>
       <c r="BG63" s="1"/>
-      <c r="BI63" s="1"/>
+      <c r="BH63" s="1"/>
       <c r="BJ63" s="1"/>
       <c r="BK63" s="1"/>
       <c r="BL63" s="1"/>
@@ -5368,6 +5483,7 @@
       <c r="BP63" s="1"/>
       <c r="BQ63" s="1"/>
       <c r="BR63" s="1"/>
+      <c r="BS63" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5386,9 +5502,9 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5405,7 +5521,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>89</v>
@@ -5417,7 +5533,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -5434,7 +5550,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -5451,7 +5567,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -5477,16 +5593,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5509,7 +5625,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -5528,7 +5644,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -5536,7 +5652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5550,7 +5666,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5570,7 +5686,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -5607,12 +5723,12 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -5626,7 +5742,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5640,7 +5756,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -5649,7 +5765,7 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -5658,7 +5774,7 @@
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -5667,7 +5783,7 @@
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -5679,7 +5795,7 @@
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -5691,7 +5807,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -5703,7 +5819,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -5712,7 +5828,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -5721,7 +5837,7 @@
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -5730,7 +5846,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -5739,7 +5855,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -5751,7 +5867,7 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -5763,7 +5879,7 @@
       </c>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -5775,7 +5891,7 @@
       </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -5798,9 +5914,9 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -5814,7 +5930,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5828,7 +5944,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -5842,7 +5958,7 @@
         <v>-52.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -5856,7 +5972,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -5870,7 +5986,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -5884,7 +6000,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -5898,7 +6014,7 @@
         <v>-20.7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -5912,7 +6028,7 @@
         <v>-52.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -5926,7 +6042,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -5940,7 +6056,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -5954,7 +6070,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updated Jupyter notebook docs for AIChE 2019
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDDCBBD-357E-4272-A1C8-DE05BB960569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C372764-55C9-4DD9-9F57-A90D608613C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2745" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="124">
   <si>
     <t>name</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Number of sites occupied by species. Leave blank for gas species. 1 for monodentate species.</t>
+  </si>
+  <si>
+    <t>Ru(0001) with atoms deleted</t>
   </si>
 </sst>
 </file>
@@ -1285,22 +1288,22 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1389,7 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1431,7 +1434,7 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>2744</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1578,7 +1581,7 @@
       <c r="G7" s="3"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1587,7 +1590,7 @@
       <c r="G8" s="3"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1596,7 +1599,7 @@
       <c r="G9" s="3"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1605,7 +1608,7 @@
       <c r="G10" s="3"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1614,7 +1617,7 @@
       <c r="G11" s="3"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1623,7 +1626,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1632,7 +1635,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1641,7 +1644,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1650,7 +1653,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1659,7 +1662,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1668,7 +1671,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1677,7 +1680,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1686,7 +1689,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1695,7 +1698,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1704,7 +1707,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1713,7 +1716,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1722,7 +1725,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1731,7 +1734,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1740,7 +1743,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1749,7 +1752,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1758,7 +1761,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1767,7 +1770,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1785,26 +1788,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1920,7 +1923,7 @@
       <c r="BR1" s="1"/>
       <c r="BS1" s="1"/>
     </row>
-    <row r="2" spans="1:71" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2036,7 +2039,7 @@
       <c r="BR2" s="1"/>
       <c r="BS2" s="1"/>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2121,7 +2124,7 @@
       <c r="BR3" s="1"/>
       <c r="BS3" s="1"/>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2215,7 +2218,7 @@
       <c r="BR4" s="1"/>
       <c r="BS4" s="1"/>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2300,7 +2303,7 @@
       <c r="BR5" s="1"/>
       <c r="BS5" s="1"/>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -2392,7 +2395,7 @@
       <c r="BR6" s="1"/>
       <c r="BS6" s="1"/>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2480,7 +2483,7 @@
       <c r="BR7" s="1"/>
       <c r="BS7" s="1"/>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2553,7 +2556,7 @@
       <c r="BR8" s="1"/>
       <c r="BS8" s="1"/>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -2647,7 +2650,7 @@
       <c r="BR9" s="1"/>
       <c r="BS9" s="1"/>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -2735,7 +2738,7 @@
       <c r="BR10" s="1"/>
       <c r="BS10" s="1"/>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -2817,7 +2820,7 @@
       <c r="BR11" s="1"/>
       <c r="BS11" s="1"/>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -2907,7 +2910,7 @@
       <c r="BR12" s="1"/>
       <c r="BS12" s="1"/>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -2991,7 +2994,7 @@
       <c r="BR13" s="1"/>
       <c r="BS13" s="1"/>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -3069,7 +3072,7 @@
       <c r="BR14" s="1"/>
       <c r="BS14" s="1"/>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -3144,7 +3147,7 @@
       <c r="BQ15" s="1"/>
       <c r="BR15" s="1"/>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -3209,7 +3212,7 @@
       <c r="BR16" s="1"/>
       <c r="BS16" s="1"/>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3288,7 +3291,7 @@
       <c r="BR17" s="1"/>
       <c r="BS17" s="1"/>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3361,7 +3364,7 @@
       <c r="BR18" s="1"/>
       <c r="BS18" s="1"/>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -3434,7 +3437,7 @@
       <c r="BR19" s="1"/>
       <c r="BS19" s="1"/>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3528,7 +3531,7 @@
       <c r="BR20" s="1"/>
       <c r="BS20" s="1"/>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -3616,7 +3619,7 @@
       <c r="BR21" s="1"/>
       <c r="BS21" s="1"/>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -3698,7 +3701,7 @@
       <c r="BR22" s="1"/>
       <c r="BS22" s="1"/>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3788,7 +3791,7 @@
       <c r="BR23" s="1"/>
       <c r="BS23" s="1"/>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3872,7 +3875,7 @@
       <c r="BR24" s="1"/>
       <c r="BS24" s="1"/>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -3950,7 +3953,7 @@
       <c r="BR25" s="1"/>
       <c r="BS25" s="1"/>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -4025,7 +4028,7 @@
       <c r="BR26" s="1"/>
       <c r="BS26" s="1"/>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -4090,7 +4093,7 @@
       <c r="BR27" s="1"/>
       <c r="BS27" s="1"/>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4155,7 +4158,7 @@
       <c r="BR28" s="1"/>
       <c r="BS28" s="1"/>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71" x14ac:dyDescent="0.3">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="AK29" s="1"/>
@@ -4193,7 +4196,7 @@
       <c r="BR29" s="1"/>
       <c r="BS29" s="1"/>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="AK30" s="1"/>
@@ -4231,7 +4234,7 @@
       <c r="BR30" s="1"/>
       <c r="BS30" s="1"/>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="AK31" s="1"/>
@@ -4269,7 +4272,7 @@
       <c r="BR31" s="1"/>
       <c r="BS31" s="1"/>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="AK32" s="1"/>
@@ -4307,7 +4310,7 @@
       <c r="BR32" s="1"/>
       <c r="BS32" s="1"/>
     </row>
-    <row r="33" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="AK33" s="1"/>
@@ -4345,7 +4348,7 @@
       <c r="BR33" s="1"/>
       <c r="BS33" s="1"/>
     </row>
-    <row r="34" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="AK34" s="1"/>
@@ -4383,7 +4386,7 @@
       <c r="BR34" s="1"/>
       <c r="BS34" s="1"/>
     </row>
-    <row r="35" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="AK35" s="1"/>
@@ -4421,7 +4424,7 @@
       <c r="BR35" s="1"/>
       <c r="BS35" s="1"/>
     </row>
-    <row r="36" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="AK36" s="1"/>
@@ -4459,7 +4462,7 @@
       <c r="BR36" s="1"/>
       <c r="BS36" s="1"/>
     </row>
-    <row r="37" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="AK37" s="1"/>
@@ -4497,7 +4500,7 @@
       <c r="BR37" s="1"/>
       <c r="BS37" s="1"/>
     </row>
-    <row r="38" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="AK38" s="1"/>
@@ -4535,7 +4538,7 @@
       <c r="BR38" s="1"/>
       <c r="BS38" s="1"/>
     </row>
-    <row r="39" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="AK39" s="1"/>
@@ -4573,7 +4576,7 @@
       <c r="BR39" s="1"/>
       <c r="BS39" s="1"/>
     </row>
-    <row r="40" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="AK40" s="1"/>
@@ -4611,7 +4614,7 @@
       <c r="BR40" s="1"/>
       <c r="BS40" s="1"/>
     </row>
-    <row r="41" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="AK41" s="1"/>
@@ -4649,7 +4652,7 @@
       <c r="BR41" s="1"/>
       <c r="BS41" s="1"/>
     </row>
-    <row r="42" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="AK42" s="1"/>
@@ -4687,7 +4690,7 @@
       <c r="BR42" s="1"/>
       <c r="BS42" s="1"/>
     </row>
-    <row r="43" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="AK43" s="1"/>
@@ -4725,7 +4728,7 @@
       <c r="BR43" s="1"/>
       <c r="BS43" s="1"/>
     </row>
-    <row r="44" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="AK44" s="1"/>
@@ -4763,7 +4766,7 @@
       <c r="BR44" s="1"/>
       <c r="BS44" s="1"/>
     </row>
-    <row r="45" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="AK45" s="1"/>
@@ -4801,7 +4804,7 @@
       <c r="BR45" s="1"/>
       <c r="BS45" s="1"/>
     </row>
-    <row r="46" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="AK46" s="1"/>
@@ -4839,7 +4842,7 @@
       <c r="BR46" s="1"/>
       <c r="BS46" s="1"/>
     </row>
-    <row r="47" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="AK47" s="1"/>
@@ -4877,7 +4880,7 @@
       <c r="BR47" s="1"/>
       <c r="BS47" s="1"/>
     </row>
-    <row r="48" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="AK48" s="1"/>
@@ -4915,7 +4918,7 @@
       <c r="BR48" s="1"/>
       <c r="BS48" s="1"/>
     </row>
-    <row r="49" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="AK49" s="1"/>
@@ -4953,7 +4956,7 @@
       <c r="BR49" s="1"/>
       <c r="BS49" s="1"/>
     </row>
-    <row r="50" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="AK50" s="1"/>
@@ -4991,7 +4994,7 @@
       <c r="BR50" s="1"/>
       <c r="BS50" s="1"/>
     </row>
-    <row r="51" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="AK51" s="1"/>
@@ -5029,7 +5032,7 @@
       <c r="BR51" s="1"/>
       <c r="BS51" s="1"/>
     </row>
-    <row r="52" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="AK52" s="1"/>
@@ -5067,7 +5070,7 @@
       <c r="BR52" s="1"/>
       <c r="BS52" s="1"/>
     </row>
-    <row r="53" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="AK53" s="1"/>
@@ -5105,7 +5108,7 @@
       <c r="BR53" s="1"/>
       <c r="BS53" s="1"/>
     </row>
-    <row r="54" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="AK54" s="1"/>
@@ -5143,7 +5146,7 @@
       <c r="BR54" s="1"/>
       <c r="BS54" s="1"/>
     </row>
-    <row r="55" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="AK55" s="1"/>
@@ -5181,7 +5184,7 @@
       <c r="BR55" s="1"/>
       <c r="BS55" s="1"/>
     </row>
-    <row r="56" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="AK56" s="1"/>
@@ -5219,7 +5222,7 @@
       <c r="BR56" s="1"/>
       <c r="BS56" s="1"/>
     </row>
-    <row r="57" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="AK57" s="1"/>
@@ -5257,7 +5260,7 @@
       <c r="BR57" s="1"/>
       <c r="BS57" s="1"/>
     </row>
-    <row r="58" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="AK58" s="1"/>
@@ -5295,7 +5298,7 @@
       <c r="BR58" s="1"/>
       <c r="BS58" s="1"/>
     </row>
-    <row r="59" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="AK59" s="1"/>
@@ -5333,7 +5336,7 @@
       <c r="BR59" s="1"/>
       <c r="BS59" s="1"/>
     </row>
-    <row r="60" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="AK60" s="1"/>
@@ -5371,7 +5374,7 @@
       <c r="BR60" s="1"/>
       <c r="BS60" s="1"/>
     </row>
-    <row r="61" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="AK61" s="1"/>
@@ -5409,7 +5412,7 @@
       <c r="BR61" s="1"/>
       <c r="BS61" s="1"/>
     </row>
-    <row r="62" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="AK62" s="1"/>
@@ -5447,7 +5450,7 @@
       <c r="BR62" s="1"/>
       <c r="BS62" s="1"/>
     </row>
-    <row r="63" spans="5:71" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:71" x14ac:dyDescent="0.3">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="AK63" s="1"/>
@@ -5495,16 +5498,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA3BA1A-334E-44D2-96CB-219546C8DBF5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5521,7 +5524,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>89</v>
@@ -5533,7 +5536,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -5550,7 +5553,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -5567,7 +5570,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -5593,16 +5596,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5625,7 +5635,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -5640,11 +5650,11 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -5652,7 +5662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5666,7 +5676,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5686,7 +5696,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -5703,7 +5713,7 @@
         <v>54</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5723,12 +5733,13 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -5742,7 +5753,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -5756,7 +5767,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -5765,7 +5776,7 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -5774,7 +5785,7 @@
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -5783,7 +5794,7 @@
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -5795,7 +5806,7 @@
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -5807,7 +5818,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -5819,7 +5830,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -5828,7 +5839,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -5837,7 +5848,7 @@
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -5846,7 +5857,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -5855,7 +5866,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -5867,7 +5878,7 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -5879,7 +5890,7 @@
       </c>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -5891,7 +5902,7 @@
       </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -5910,41 +5921,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -5958,7 +5972,7 @@
         <v>-52.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -5972,7 +5986,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -5986,7 +6000,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -6000,7 +6014,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -6014,7 +6028,7 @@
         <v>-20.7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6028,7 +6042,7 @@
         <v>-52.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -6042,7 +6056,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -6056,7 +6070,7 @@
         <v>-17.7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -6070,7 +6084,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Improved documentation for new release.
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -1,31 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox (Personal)\UDel Documents (Dropbox)\UDel Research\Github\pMuTT_development\docs\source\examples_jupyter\omkm_io\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_dev\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC11594-A9ED-417C-8314-36B7B26A8866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A29F855-D91C-4F59-9343-BD912016FAC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="576" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
     <sheet name="species" sheetId="1" r:id="rId2"/>
-    <sheet name="beps" sheetId="7" r:id="rId3"/>
-    <sheet name="phases" sheetId="5" r:id="rId4"/>
-    <sheet name="reactions" sheetId="3" r:id="rId5"/>
-    <sheet name="lateral_interactions" sheetId="6" r:id="rId6"/>
+    <sheet name="reactor" sheetId="8" r:id="rId3"/>
+    <sheet name="units" sheetId="9" r:id="rId4"/>
+    <sheet name="beps" sheetId="7" r:id="rId5"/>
+    <sheet name="phases" sheetId="5" r:id="rId6"/>
+    <sheet name="reactions" sheetId="3" r:id="rId7"/>
+    <sheet name="lateral_interactions" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -287,12 +291,6 @@
     <t>direction</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Optional name to give to reaction</t>
-  </si>
-  <si>
     <t>N-H</t>
   </si>
   <si>
@@ -414,6 +412,177 @@
   </si>
   <si>
     <t>dict.initial_state.NH3</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>Temperature exponent for rate constant expression. Typically 0 for adsorption reactions and 1 for surface reactions</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>T_low</t>
+  </si>
+  <si>
+    <t>T_high</t>
+  </si>
+  <si>
+    <t>Lower temperature bound to use for NASA polynomial fit</t>
+  </si>
+  <si>
+    <t>Upper temperature bound to use for NASA polynomial fit</t>
+  </si>
+  <si>
+    <t>reactor_type</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>cat_abyv</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>flow_rate</t>
+  </si>
+  <si>
+    <t>transient</t>
+  </si>
+  <si>
+    <t>stepping</t>
+  </si>
+  <si>
+    <t>init_step</t>
+  </si>
+  <si>
+    <t>atol</t>
+  </si>
+  <si>
+    <t>rtol</t>
+  </si>
+  <si>
+    <t>output_format</t>
+  </si>
+  <si>
+    <t>cstr</t>
+  </si>
+  <si>
+    <t>isothermal</t>
+  </si>
+  <si>
+    <t>logarithmic</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>Type of reactor. Accepted options include 'pfr', 'cstr', 'pfr_0d', 'batch'</t>
+  </si>
+  <si>
+    <t>Mode of operation.</t>
+  </si>
+  <si>
+    <t>Volume of reactor (units correspond to length^3 in units sheet)</t>
+  </si>
+  <si>
+    <t>Temperature of reactor in K</t>
+  </si>
+  <si>
+    <t>Pressure of reactor (units correspond to pressure in units sheet)</t>
+  </si>
+  <si>
+    <t>Catalyst surface area to reactor volume ratio (units correspond to 1/length in units sheet)</t>
+  </si>
+  <si>
+    <t>Time taken to converge (units correspond to time in unit sheet)</t>
+  </si>
+  <si>
+    <t>Flow rate (units correspond to length^3/time in units sheet)</t>
+  </si>
+  <si>
+    <t>If True, transient run data will be saved.</t>
+  </si>
+  <si>
+    <t>Type of time stepping to perform during transient runs.</t>
+  </si>
+  <si>
+    <t>Solver option for initial time step taken. Corresponds to time in units sheet.</t>
+  </si>
+  <si>
+    <t>Solver option for absolute tolerance.</t>
+  </si>
+  <si>
+    <t>Solver option for relative tolerance</t>
+  </si>
+  <si>
+    <t>Format to write output formats. Accepted options are 'dat' and 'csv'.</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>act_energy</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>Units for length</t>
+  </si>
+  <si>
+    <t>Units for quantity</t>
+  </si>
+  <si>
+    <t>Units for activation energy</t>
+  </si>
+  <si>
+    <t>Units for mass</t>
+  </si>
+  <si>
+    <t>Units for energies not related to activation energy</t>
+  </si>
+  <si>
+    <t>Units for pressure</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>mol</t>
+  </si>
+  <si>
+    <t>kcal/mol</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>atm</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1463,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,13 +1964,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BS63"/>
+  <dimension ref="A1:BU63"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,13 +1979,13 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1833,25 +2002,25 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>51</v>
@@ -1883,11 +2052,15 @@
       <c r="V1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="W1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
@@ -1931,8 +2104,10 @@
       <c r="BQ1" s="1"/>
       <c r="BR1" s="1"/>
       <c r="BS1" s="1"/>
-    </row>
-    <row r="2" spans="1:71" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BT1" s="1"/>
+      <c r="BU1" s="1"/>
+    </row>
+    <row r="2" spans="1:73" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1949,25 +2124,25 @@
         <v>55</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>19</v>
@@ -1999,11 +2174,15 @@
       <c r="V2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
+      <c r="W2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
@@ -2047,8 +2226,10 @@
       <c r="BQ2" s="1"/>
       <c r="BR2" s="1"/>
       <c r="BS2" s="1"/>
-    </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+    </row>
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2058,37 +2239,41 @@
       <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>300</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="4">
+      <c r="L3" s="4">
         <v>-16.63</v>
       </c>
-      <c r="K3" s="4">
+      <c r="M3" s="4">
         <v>2744</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
       <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
@@ -2132,8 +2317,10 @@
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
       <c r="BS3" s="1"/>
-    </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
+    </row>
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2146,43 +2333,47 @@
       <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>300</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="4">
+      <c r="L4" s="4">
         <v>-19.54</v>
       </c>
-      <c r="K4" s="4">
+      <c r="M4" s="4">
         <v>3534</v>
       </c>
-      <c r="L4" s="4">
+      <c r="N4" s="4">
         <v>3464</v>
       </c>
-      <c r="M4" s="4">
+      <c r="O4" s="4">
         <v>1765</v>
       </c>
-      <c r="N4" s="4">
+      <c r="P4" s="4">
         <v>1139</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
       <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
@@ -2226,8 +2417,10 @@
       <c r="BQ4" s="1"/>
       <c r="BR4" s="1"/>
       <c r="BS4" s="1"/>
-    </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT4" s="1"/>
+      <c r="BU4" s="1"/>
+    </row>
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2237,37 +2430,41 @@
       <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>300</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="4">
+      <c r="L5" s="4">
         <v>-6.77</v>
       </c>
-      <c r="K5" s="4">
+      <c r="M5" s="4">
         <v>4342</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
       <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
@@ -2311,10 +2508,12 @@
       <c r="BQ5" s="1"/>
       <c r="BR5" s="1"/>
       <c r="BS5" s="1"/>
-    </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT5" s="1"/>
+      <c r="BU5" s="1"/>
+    </row>
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2325,41 +2524,45 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>300</v>
+      </c>
+      <c r="H6">
+        <v>1000</v>
+      </c>
+      <c r="I6" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="4">
+      <c r="L6" s="4">
         <v>-17.239999999999952</v>
       </c>
-      <c r="K6" s="4">
+      <c r="M6" s="4">
         <v>2197.19</v>
       </c>
-      <c r="L6" s="4">
+      <c r="N6" s="4">
         <v>360.41500000000002</v>
       </c>
-      <c r="M6" s="4">
+      <c r="O6" s="4">
         <v>347.34300000000002</v>
       </c>
-      <c r="N6" s="4">
+      <c r="P6" s="4">
         <v>335.67399999999998</v>
       </c>
-      <c r="O6" s="4">
+      <c r="Q6" s="4">
         <v>62.076000000000001</v>
       </c>
-      <c r="P6" s="4">
+      <c r="R6" s="4">
         <v>32.179400000000001</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
       <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
@@ -2403,10 +2606,12 @@
       <c r="BQ6" s="1"/>
       <c r="BR6" s="1"/>
       <c r="BS6" s="1"/>
-    </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
+    </row>
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2417,39 +2622,43 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>300</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="4">
+      <c r="L7" s="4">
         <v>-9.339999999999975</v>
       </c>
-      <c r="K7" s="4">
+      <c r="M7" s="4">
         <v>549.10500000000002</v>
       </c>
-      <c r="L7" s="4">
+      <c r="N7" s="4">
         <v>538.55999999999995</v>
       </c>
-      <c r="M7" s="4">
+      <c r="O7" s="4">
         <v>504.32299999999998</v>
       </c>
-      <c r="N7" s="4">
+      <c r="P7" s="4">
         <v>475.80500000000001</v>
       </c>
-      <c r="O7" s="4">
+      <c r="Q7" s="4">
         <v>459.08100000000002</v>
       </c>
-      <c r="P7" s="4">
+      <c r="R7" s="4">
         <v>410.01799999999997</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-      <c r="W7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="1"/>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
@@ -2481,8 +2690,8 @@
       <c r="BF7" s="1"/>
       <c r="BG7" s="1"/>
       <c r="BH7" s="1"/>
+      <c r="BI7" s="1"/>
       <c r="BJ7" s="1"/>
-      <c r="BK7" s="1"/>
       <c r="BL7" s="1"/>
       <c r="BM7" s="1"/>
       <c r="BN7" s="1"/>
@@ -2491,10 +2700,12 @@
       <c r="BQ7" s="1"/>
       <c r="BR7" s="1"/>
       <c r="BS7" s="1"/>
-    </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT7" s="1"/>
+      <c r="BU7" s="1"/>
+    </row>
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2505,23 +2716,27 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>300</v>
+      </c>
+      <c r="H8">
+        <v>1000</v>
+      </c>
+      <c r="I8" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="4">
+      <c r="L8" s="4">
         <v>-4</v>
       </c>
-      <c r="K8" s="4">
+      <c r="M8" s="4">
         <v>1003.51</v>
       </c>
-      <c r="L8" s="4">
+      <c r="N8" s="4">
         <v>625.54999999999995</v>
       </c>
-      <c r="M8" s="4">
+      <c r="O8" s="4">
         <v>616.29</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -2529,9 +2744,9 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-      <c r="W8" s="1"/>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="1"/>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
@@ -2554,8 +2769,8 @@
       <c r="BF8" s="1"/>
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
       <c r="BJ8" s="1"/>
-      <c r="BK8" s="1"/>
       <c r="BL8" s="1"/>
       <c r="BM8" s="1"/>
       <c r="BN8" s="1"/>
@@ -2564,10 +2779,12 @@
       <c r="BQ8" s="1"/>
       <c r="BR8" s="1"/>
       <c r="BS8" s="1"/>
-    </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT8" s="1"/>
+      <c r="BU8" s="1"/>
+    </row>
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2581,51 +2798,55 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <v>300</v>
+      </c>
+      <c r="H9">
+        <v>1000</v>
+      </c>
+      <c r="I9" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="4">
+      <c r="L9" s="4">
         <v>-20.42999999999995</v>
       </c>
-      <c r="K9" s="4">
+      <c r="M9" s="4">
         <v>3491.0891299999998</v>
       </c>
-      <c r="L9" s="4">
+      <c r="N9" s="4">
         <v>3488.8194899999999</v>
       </c>
-      <c r="M9" s="4">
+      <c r="O9" s="4">
         <v>3364.5232299999998</v>
       </c>
-      <c r="N9" s="4">
+      <c r="P9" s="4">
         <v>1583.5157099999999</v>
       </c>
-      <c r="O9" s="4">
+      <c r="Q9" s="4">
         <v>1582.0703000000001</v>
       </c>
-      <c r="P9" s="4">
+      <c r="R9" s="4">
         <v>1124.22477</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="S9" s="4">
         <v>570.21231</v>
       </c>
-      <c r="R9" s="4">
+      <c r="T9" s="4">
         <v>567.22147099999995</v>
       </c>
-      <c r="S9" s="4">
+      <c r="U9" s="4">
         <v>333.08962400000001</v>
       </c>
-      <c r="T9" s="4">
+      <c r="V9" s="4">
         <v>122.859345</v>
       </c>
-      <c r="U9" s="4">
+      <c r="W9" s="4">
         <v>83.828554999999994</v>
       </c>
-      <c r="V9" s="4">
+      <c r="X9" s="4">
         <v>70.625114999999994</v>
       </c>
-      <c r="W9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
+      <c r="Y9" s="1"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
@@ -2648,8 +2869,8 @@
       <c r="BF9" s="1"/>
       <c r="BG9" s="1"/>
       <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
       <c r="BJ9" s="1"/>
-      <c r="BK9" s="1"/>
       <c r="BL9" s="1"/>
       <c r="BM9" s="1"/>
       <c r="BN9" s="1"/>
@@ -2658,10 +2879,12 @@
       <c r="BQ9" s="1"/>
       <c r="BR9" s="1"/>
       <c r="BS9" s="1"/>
-    </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT9" s="1"/>
+      <c r="BU9" s="1"/>
+    </row>
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2675,45 +2898,49 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>300</v>
+      </c>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="4">
+      <c r="L10" s="4">
         <v>-16.589999999999975</v>
       </c>
-      <c r="K10" s="4">
+      <c r="M10" s="4">
         <v>3469.3003399999998</v>
       </c>
-      <c r="L10" s="4">
+      <c r="N10" s="4">
         <v>3381.05197</v>
       </c>
-      <c r="M10" s="4">
+      <c r="O10" s="4">
         <v>1503.01629</v>
       </c>
-      <c r="N10" s="4">
+      <c r="P10" s="4">
         <v>698.86880399999995</v>
       </c>
-      <c r="O10" s="4">
+      <c r="Q10" s="4">
         <v>625.59609399999999</v>
       </c>
-      <c r="P10" s="4">
+      <c r="R10" s="4">
         <v>615.93978300000003</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="S10" s="4">
         <v>475.130224</v>
       </c>
-      <c r="R10" s="4">
+      <c r="T10" s="4">
         <v>298.12000999999998</v>
       </c>
-      <c r="S10" s="4">
+      <c r="U10" s="4">
         <v>153.25013899999999</v>
       </c>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-      <c r="W10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="1"/>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
@@ -2736,8 +2963,8 @@
       <c r="BF10" s="1"/>
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
       <c r="BJ10" s="1"/>
-      <c r="BK10" s="1"/>
       <c r="BL10" s="1"/>
       <c r="BM10" s="1"/>
       <c r="BN10" s="1"/>
@@ -2746,10 +2973,12 @@
       <c r="BQ10" s="1"/>
       <c r="BR10" s="1"/>
       <c r="BS10" s="1"/>
-    </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT10" s="1"/>
+      <c r="BU10" s="1"/>
+    </row>
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2763,39 +2992,43 @@
       <c r="F11">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>300</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="4">
+      <c r="L11" s="4">
         <v>-13.20999999999998</v>
       </c>
-      <c r="K11" s="4">
+      <c r="M11" s="4">
         <v>3403.12878</v>
       </c>
-      <c r="L11" s="4">
+      <c r="N11" s="4">
         <v>718.17758800000001</v>
       </c>
-      <c r="M11" s="4">
+      <c r="O11" s="4">
         <v>710.58051999999998</v>
       </c>
-      <c r="N11" s="4">
+      <c r="P11" s="4">
         <v>528.52565900000002</v>
       </c>
-      <c r="O11" s="4">
+      <c r="Q11" s="4">
         <v>415.19586900000002</v>
       </c>
-      <c r="P11" s="4">
+      <c r="R11" s="4">
         <v>410.13079699999997</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
-      <c r="W11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="1"/>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
@@ -2818,8 +3051,8 @@
       <c r="BF11" s="1"/>
       <c r="BG11" s="1"/>
       <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
       <c r="BJ11" s="1"/>
-      <c r="BK11" s="1"/>
       <c r="BL11" s="1"/>
       <c r="BM11" s="1"/>
       <c r="BN11" s="1"/>
@@ -2828,10 +3061,12 @@
       <c r="BQ11" s="1"/>
       <c r="BR11" s="1"/>
       <c r="BS11" s="1"/>
-    </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT11" s="1"/>
+      <c r="BU11" s="1"/>
+    </row>
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2842,50 +3077,54 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>300</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="4">
-        <f>J9+1.19</f>
+      <c r="L12" s="4">
+        <f>L9+1.19</f>
         <v>-19.239999999999949</v>
       </c>
-      <c r="K12" s="4">
+      <c r="M12" s="4">
         <v>3453.4106299999999</v>
       </c>
-      <c r="L12" s="4">
+      <c r="N12" s="4">
         <v>3355.6699199999998</v>
       </c>
-      <c r="M12" s="4">
+      <c r="O12" s="4">
         <v>1723.84977</v>
       </c>
-      <c r="N12" s="4">
+      <c r="P12" s="4">
         <v>1487.9548400000001</v>
       </c>
-      <c r="O12" s="4">
+      <c r="Q12" s="4">
         <v>959.15072299999997</v>
       </c>
-      <c r="P12" s="4">
+      <c r="R12" s="4">
         <v>888.94619799999998</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="S12" s="4">
         <v>594.08943899999997</v>
       </c>
-      <c r="R12" s="4">
+      <c r="T12" s="4">
         <v>428.43113599999998</v>
       </c>
-      <c r="S12" s="4">
+      <c r="U12" s="4">
         <v>227.032386</v>
       </c>
-      <c r="T12" s="4">
+      <c r="V12" s="4">
         <v>206.046727</v>
       </c>
-      <c r="U12" s="4">
+      <c r="W12" s="4">
         <v>142.13585599999999</v>
       </c>
-      <c r="V12" s="4"/>
-      <c r="W12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="1"/>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
@@ -2908,8 +3147,8 @@
       <c r="BF12" s="1"/>
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
+      <c r="BI12" s="1"/>
       <c r="BJ12" s="1"/>
-      <c r="BK12" s="1"/>
       <c r="BL12" s="1"/>
       <c r="BM12" s="1"/>
       <c r="BN12" s="1"/>
@@ -2918,10 +3157,12 @@
       <c r="BQ12" s="1"/>
       <c r="BR12" s="1"/>
       <c r="BS12" s="1"/>
-    </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT12" s="1"/>
+      <c r="BU12" s="1"/>
+    </row>
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2932,44 +3173,48 @@
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <v>300</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="4">
-        <f>J10+0.72</f>
+      <c r="L13" s="4">
+        <f>L10+0.72</f>
         <v>-15.869999999999974</v>
       </c>
-      <c r="K13" s="4">
+      <c r="M13" s="4">
         <v>3426.4448400000001</v>
       </c>
-      <c r="L13" s="4">
+      <c r="N13" s="4">
         <v>1293.72327</v>
       </c>
-      <c r="M13" s="4">
+      <c r="O13" s="4">
         <v>922.83076800000003</v>
       </c>
-      <c r="N13" s="4">
+      <c r="P13" s="4">
         <v>660.96659799999998</v>
       </c>
-      <c r="O13" s="4">
+      <c r="Q13" s="4">
         <v>525.59512400000006</v>
       </c>
-      <c r="P13" s="4">
+      <c r="R13" s="4">
         <v>496.83726300000001</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="S13" s="4">
         <v>330.67445900000001</v>
       </c>
-      <c r="R13" s="4">
+      <c r="T13" s="4">
         <v>290.27800500000001</v>
       </c>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
-      <c r="W13" s="1"/>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="1"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
@@ -2992,8 +3237,8 @@
       <c r="BF13" s="1"/>
       <c r="BG13" s="1"/>
       <c r="BH13" s="1"/>
+      <c r="BI13" s="1"/>
       <c r="BJ13" s="1"/>
-      <c r="BK13" s="1"/>
       <c r="BL13" s="1"/>
       <c r="BM13" s="1"/>
       <c r="BN13" s="1"/>
@@ -3002,10 +3247,12 @@
       <c r="BQ13" s="1"/>
       <c r="BR13" s="1"/>
       <c r="BS13" s="1"/>
-    </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT13" s="1"/>
+      <c r="BU13" s="1"/>
+    </row>
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3016,38 +3263,42 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14">
+        <v>1000</v>
+      </c>
+      <c r="I14" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="4">
-        <f>J11+1.28</f>
+      <c r="L14" s="4">
+        <f>L11+1.28</f>
         <v>-11.92999999999998</v>
       </c>
-      <c r="K14" s="4">
+      <c r="M14" s="4">
         <v>1201.6048699999999</v>
       </c>
-      <c r="L14" s="4">
+      <c r="N14" s="4">
         <v>491.566416</v>
       </c>
-      <c r="M14" s="4">
+      <c r="O14" s="4">
         <v>462.01550200000003</v>
       </c>
-      <c r="N14" s="4">
+      <c r="P14" s="4">
         <v>402.15890400000001</v>
       </c>
-      <c r="O14" s="4">
+      <c r="Q14" s="4">
         <v>242.13872599999999</v>
       </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-      <c r="W14" s="1"/>
-      <c r="AK14" s="1"/>
-      <c r="AL14" s="1"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="1"/>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
@@ -3070,8 +3321,8 @@
       <c r="BF14" s="1"/>
       <c r="BG14" s="1"/>
       <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
       <c r="BJ14" s="1"/>
-      <c r="BK14" s="1"/>
       <c r="BL14" s="1"/>
       <c r="BM14" s="1"/>
       <c r="BN14" s="1"/>
@@ -3080,10 +3331,12 @@
       <c r="BQ14" s="1"/>
       <c r="BR14" s="1"/>
       <c r="BS14" s="1"/>
-    </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT14" s="1"/>
+      <c r="BU14" s="1"/>
+    </row>
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3091,38 +3344,42 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>300</v>
+      </c>
+      <c r="H15">
+        <v>1000</v>
+      </c>
+      <c r="I15" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="4">
-        <f>J6+2.57</f>
+      <c r="L15" s="4">
+        <f>L6+2.57</f>
         <v>-14.669999999999952</v>
       </c>
-      <c r="K15" s="4">
+      <c r="M15" s="4">
         <v>485.61399999999998</v>
       </c>
-      <c r="L15" s="4">
+      <c r="N15" s="4">
         <v>392.97699999999998</v>
       </c>
-      <c r="M15" s="4">
+      <c r="O15" s="4">
         <v>386.18599999999998</v>
       </c>
-      <c r="N15" s="4">
+      <c r="P15" s="4">
         <v>280.94299999999998</v>
       </c>
-      <c r="O15" s="4">
+      <c r="Q15" s="4">
         <v>168.43100000000001</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-      <c r="W15" s="1"/>
-      <c r="AJ15" s="1"/>
-      <c r="AK15" s="1"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="1"/>
       <c r="AL15" s="1"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
@@ -3145,8 +3402,8 @@
       <c r="BE15" s="1"/>
       <c r="BF15" s="1"/>
       <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
       <c r="BI15" s="1"/>
-      <c r="BJ15" s="1"/>
       <c r="BK15" s="1"/>
       <c r="BL15" s="1"/>
       <c r="BM15" s="1"/>
@@ -3155,10 +3412,12 @@
       <c r="BP15" s="1"/>
       <c r="BQ15" s="1"/>
       <c r="BR15" s="1"/>
-    </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BS15" s="1"/>
+      <c r="BT15" s="1"/>
+    </row>
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3169,11 +3428,15 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <v>300</v>
+      </c>
+      <c r="H16">
+        <v>1000</v>
+      </c>
+      <c r="I16" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -3185,9 +3448,9 @@
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-      <c r="W16" s="1"/>
-      <c r="AK16" s="1"/>
-      <c r="AL16" s="1"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="1"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
@@ -3210,8 +3473,8 @@
       <c r="BF16" s="1"/>
       <c r="BG16" s="1"/>
       <c r="BH16" s="1"/>
+      <c r="BI16" s="1"/>
       <c r="BJ16" s="1"/>
-      <c r="BK16" s="1"/>
       <c r="BL16" s="1"/>
       <c r="BM16" s="1"/>
       <c r="BN16" s="1"/>
@@ -3220,8 +3483,10 @@
       <c r="BQ16" s="1"/>
       <c r="BR16" s="1"/>
       <c r="BS16" s="1"/>
-    </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT16" s="1"/>
+      <c r="BU16" s="1"/>
+    </row>
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3229,44 +3494,48 @@
         <v>2</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17">
+        <v>300</v>
+      </c>
+      <c r="H17">
+        <v>1000</v>
+      </c>
+      <c r="I17" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4">
         <v>-17.389999999999986</v>
       </c>
-      <c r="K17" s="4">
+      <c r="M17" s="4">
         <v>1015.734101</v>
       </c>
-      <c r="L17" s="4">
+      <c r="N17" s="4">
         <v>456.07363700000002</v>
       </c>
-      <c r="M17" s="4">
+      <c r="O17" s="4">
         <v>408.12729300000001</v>
       </c>
-      <c r="N17" s="4">
+      <c r="P17" s="4">
         <v>378.51690000000002</v>
       </c>
-      <c r="O17" s="4">
+      <c r="Q17" s="4">
         <v>344.87134400000002</v>
       </c>
-      <c r="P17" s="4">
+      <c r="R17" s="4">
         <v>334.62168200000002</v>
       </c>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-      <c r="AK17" s="1"/>
-      <c r="AL17" s="1"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
@@ -3289,8 +3558,8 @@
       <c r="BF17" s="1"/>
       <c r="BG17" s="1"/>
       <c r="BH17" s="1"/>
+      <c r="BI17" s="1"/>
       <c r="BJ17" s="1"/>
-      <c r="BK17" s="1"/>
       <c r="BL17" s="1"/>
       <c r="BM17" s="1"/>
       <c r="BN17" s="1"/>
@@ -3299,8 +3568,10 @@
       <c r="BQ17" s="1"/>
       <c r="BR17" s="1"/>
       <c r="BS17" s="1"/>
-    </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT17" s="1"/>
+      <c r="BU17" s="1"/>
+    </row>
+    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3308,29 +3579,33 @@
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18">
+        <v>300</v>
+      </c>
+      <c r="H18">
+        <v>1000</v>
+      </c>
+      <c r="I18" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4">
         <v>-9.3899999999999864</v>
       </c>
-      <c r="K18" s="4">
+      <c r="M18" s="4">
         <v>529.80737599999998</v>
       </c>
-      <c r="L18" s="4">
+      <c r="N18" s="4">
         <v>506.95443399999999</v>
       </c>
-      <c r="M18" s="4">
+      <c r="O18" s="4">
         <v>471.09772600000002</v>
       </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -3338,8 +3613,8 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
-      <c r="AK18" s="1"/>
-      <c r="AL18" s="1"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
@@ -3362,8 +3637,8 @@
       <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
+      <c r="BI18" s="1"/>
       <c r="BJ18" s="1"/>
-      <c r="BK18" s="1"/>
       <c r="BL18" s="1"/>
       <c r="BM18" s="1"/>
       <c r="BN18" s="1"/>
@@ -3372,8 +3647,10 @@
       <c r="BQ18" s="1"/>
       <c r="BR18" s="1"/>
       <c r="BS18" s="1"/>
-    </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT18" s="1"/>
+      <c r="BU18" s="1"/>
+    </row>
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -3381,29 +3658,33 @@
         <v>1</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19">
+        <v>300</v>
+      </c>
+      <c r="H19">
+        <v>1000</v>
+      </c>
+      <c r="I19" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4">
         <v>-4</v>
       </c>
-      <c r="K19" s="4">
+      <c r="M19" s="4">
         <v>1003.51</v>
       </c>
-      <c r="L19" s="4">
+      <c r="N19" s="4">
         <v>625.54999999999995</v>
       </c>
-      <c r="M19" s="4">
+      <c r="O19" s="4">
         <v>616.29</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -3411,8 +3692,8 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-      <c r="AK19" s="1"/>
-      <c r="AL19" s="1"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
@@ -3435,8 +3716,8 @@
       <c r="BF19" s="1"/>
       <c r="BG19" s="1"/>
       <c r="BH19" s="1"/>
+      <c r="BI19" s="1"/>
       <c r="BJ19" s="1"/>
-      <c r="BK19" s="1"/>
       <c r="BL19" s="1"/>
       <c r="BM19" s="1"/>
       <c r="BN19" s="1"/>
@@ -3445,8 +3726,10 @@
       <c r="BQ19" s="1"/>
       <c r="BR19" s="1"/>
       <c r="BS19" s="1"/>
-    </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT19" s="1"/>
+      <c r="BU19" s="1"/>
+    </row>
+    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3457,56 +3740,60 @@
         <v>3</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <v>300</v>
+      </c>
+      <c r="H20">
+        <v>1000</v>
+      </c>
+      <c r="I20" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4">
+      <c r="K20" s="4"/>
+      <c r="L20" s="4">
         <v>-20.67999999999995</v>
       </c>
-      <c r="K20" s="4">
+      <c r="M20" s="4">
         <v>3498.0269910000002</v>
       </c>
-      <c r="L20" s="4">
+      <c r="N20" s="4">
         <v>3469.3304969999999</v>
       </c>
-      <c r="M20" s="4">
+      <c r="O20" s="4">
         <v>3362.813486</v>
       </c>
-      <c r="N20" s="4">
+      <c r="P20" s="4">
         <v>1590.9105280000001</v>
       </c>
-      <c r="O20" s="4">
+      <c r="Q20" s="4">
         <v>1579.266171</v>
       </c>
-      <c r="P20" s="4">
+      <c r="R20" s="4">
         <v>1140.7628299999999</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="S20" s="4">
         <v>564.97479799999996</v>
       </c>
-      <c r="R20" s="4">
+      <c r="T20" s="4">
         <v>555.49956799999995</v>
       </c>
-      <c r="S20" s="4">
+      <c r="U20" s="4">
         <v>336.10022600000002</v>
       </c>
-      <c r="T20" s="4">
+      <c r="V20" s="4">
         <v>117.161717</v>
       </c>
-      <c r="U20" s="4">
+      <c r="W20" s="4">
         <v>86.774373999999995</v>
       </c>
-      <c r="V20" s="4">
+      <c r="X20" s="4">
         <v>78.100128999999995</v>
       </c>
-      <c r="AK20" s="1"/>
-      <c r="AL20" s="1"/>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
@@ -3529,8 +3816,8 @@
       <c r="BF20" s="1"/>
       <c r="BG20" s="1"/>
       <c r="BH20" s="1"/>
+      <c r="BI20" s="1"/>
       <c r="BJ20" s="1"/>
-      <c r="BK20" s="1"/>
       <c r="BL20" s="1"/>
       <c r="BM20" s="1"/>
       <c r="BN20" s="1"/>
@@ -3539,8 +3826,10 @@
       <c r="BQ20" s="1"/>
       <c r="BR20" s="1"/>
       <c r="BS20" s="1"/>
-    </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT20" s="1"/>
+      <c r="BU20" s="1"/>
+    </row>
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -3551,50 +3840,54 @@
         <v>2</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21">
+        <v>300</v>
+      </c>
+      <c r="H21">
+        <v>1000</v>
+      </c>
+      <c r="I21" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4">
         <v>-17.149999999999977</v>
       </c>
-      <c r="K21" s="4">
+      <c r="M21" s="4">
         <v>3528.6824689999999</v>
       </c>
-      <c r="L21" s="4">
+      <c r="N21" s="4">
         <v>3375.447388</v>
       </c>
-      <c r="M21" s="4">
+      <c r="O21" s="4">
         <v>1477.164</v>
       </c>
-      <c r="N21" s="4">
+      <c r="P21" s="4">
         <v>720.07573000000002</v>
       </c>
-      <c r="O21" s="4">
+      <c r="Q21" s="4">
         <v>615.66630499999997</v>
       </c>
-      <c r="P21" s="4">
+      <c r="R21" s="4">
         <v>581.96669099999997</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="S21" s="4">
         <v>468.85326900000001</v>
       </c>
-      <c r="R21" s="4">
+      <c r="T21" s="4">
         <v>286.369823</v>
       </c>
-      <c r="S21" s="4">
+      <c r="U21" s="4">
         <v>105.95658400000001</v>
       </c>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="AK21" s="1"/>
-      <c r="AL21" s="1"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
@@ -3617,8 +3910,8 @@
       <c r="BF21" s="1"/>
       <c r="BG21" s="1"/>
       <c r="BH21" s="1"/>
+      <c r="BI21" s="1"/>
       <c r="BJ21" s="1"/>
-      <c r="BK21" s="1"/>
       <c r="BL21" s="1"/>
       <c r="BM21" s="1"/>
       <c r="BN21" s="1"/>
@@ -3627,8 +3920,10 @@
       <c r="BQ21" s="1"/>
       <c r="BR21" s="1"/>
       <c r="BS21" s="1"/>
-    </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT21" s="1"/>
+      <c r="BU21" s="1"/>
+    </row>
+    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -3639,44 +3934,48 @@
         <v>1</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22">
+        <v>300</v>
+      </c>
+      <c r="H22">
+        <v>1000</v>
+      </c>
+      <c r="I22" t="s">
         <v>3</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4">
+      <c r="K22" s="4"/>
+      <c r="L22" s="4">
         <v>-13.1099999999999</v>
       </c>
-      <c r="K22" s="4">
+      <c r="M22" s="4">
         <v>3384.3746510000001</v>
       </c>
-      <c r="L22" s="4">
+      <c r="N22" s="4">
         <v>726.230954</v>
       </c>
-      <c r="M22" s="4">
+      <c r="O22" s="4">
         <v>669.42910800000004</v>
       </c>
-      <c r="N22" s="4">
+      <c r="P22" s="4">
         <v>506.27813500000002</v>
       </c>
-      <c r="O22" s="4">
+      <c r="Q22" s="4">
         <v>409.50201399999997</v>
       </c>
-      <c r="P22" s="4">
+      <c r="R22" s="4">
         <v>387.80818099999999</v>
       </c>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-      <c r="AK22" s="1"/>
-      <c r="AL22" s="1"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
@@ -3699,8 +3998,8 @@
       <c r="BF22" s="1"/>
       <c r="BG22" s="1"/>
       <c r="BH22" s="1"/>
+      <c r="BI22" s="1"/>
       <c r="BJ22" s="1"/>
-      <c r="BK22" s="1"/>
       <c r="BL22" s="1"/>
       <c r="BM22" s="1"/>
       <c r="BN22" s="1"/>
@@ -3709,8 +4008,10 @@
       <c r="BQ22" s="1"/>
       <c r="BR22" s="1"/>
       <c r="BS22" s="1"/>
-    </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT22" s="1"/>
+      <c r="BU22" s="1"/>
+    </row>
+    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -3724,49 +4025,53 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23">
+        <v>300</v>
+      </c>
+      <c r="H23">
+        <v>1000</v>
+      </c>
+      <c r="I23" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4">
         <v>-19.809999999999945</v>
       </c>
-      <c r="K23" s="4">
+      <c r="M23" s="4">
         <v>3484.3961949999998</v>
       </c>
-      <c r="L23" s="4">
+      <c r="N23" s="4">
         <v>3385.2659090000002</v>
       </c>
-      <c r="M23" s="4">
+      <c r="O23" s="4">
         <v>1685.8293080000001</v>
       </c>
-      <c r="N23" s="4">
+      <c r="P23" s="4">
         <v>1480.998257</v>
       </c>
-      <c r="O23" s="4">
+      <c r="Q23" s="4">
         <v>1002.067555</v>
       </c>
-      <c r="P23" s="4">
+      <c r="R23" s="4">
         <v>916.14745100000005</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="S23" s="4">
         <v>575.40527899999995</v>
       </c>
-      <c r="R23" s="4">
+      <c r="T23" s="4">
         <v>431.30664400000001</v>
       </c>
-      <c r="S23" s="4">
+      <c r="U23" s="4">
         <v>345.148708</v>
       </c>
-      <c r="T23" s="4">
+      <c r="V23" s="4">
         <v>221.64965799999999</v>
       </c>
-      <c r="U23" s="4">
+      <c r="W23" s="4">
         <v>70.339661000000007</v>
       </c>
-      <c r="V23" s="4"/>
-      <c r="AK23" s="1"/>
-      <c r="AL23" s="1"/>
+      <c r="X23" s="4"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
@@ -3789,8 +4094,8 @@
       <c r="BF23" s="1"/>
       <c r="BG23" s="1"/>
       <c r="BH23" s="1"/>
+      <c r="BI23" s="1"/>
       <c r="BJ23" s="1"/>
-      <c r="BK23" s="1"/>
       <c r="BL23" s="1"/>
       <c r="BM23" s="1"/>
       <c r="BN23" s="1"/>
@@ -3799,8 +4104,10 @@
       <c r="BQ23" s="1"/>
       <c r="BR23" s="1"/>
       <c r="BS23" s="1"/>
-    </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT23" s="1"/>
+      <c r="BU23" s="1"/>
+    </row>
+    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3814,43 +4121,47 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24">
+        <v>300</v>
+      </c>
+      <c r="H24">
+        <v>1000</v>
+      </c>
+      <c r="I24" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4">
+      <c r="K24" s="4"/>
+      <c r="L24" s="4">
         <v>-15.819999999999936</v>
       </c>
-      <c r="K24" s="4">
+      <c r="M24" s="4">
         <v>3432.815967</v>
       </c>
-      <c r="L24" s="4">
+      <c r="N24" s="4">
         <v>1789.8865699999999</v>
       </c>
-      <c r="M24" s="4">
+      <c r="O24" s="4">
         <v>1032.1897269999999</v>
       </c>
-      <c r="N24" s="4">
+      <c r="P24" s="4">
         <v>583.47939799999995</v>
       </c>
-      <c r="O24" s="4">
+      <c r="Q24" s="4">
         <v>392.83707299999998</v>
       </c>
-      <c r="P24" s="4">
+      <c r="R24" s="4">
         <v>384.833597</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="S24" s="4">
         <v>311.60087600000003</v>
       </c>
-      <c r="R24" s="4">
+      <c r="T24" s="4">
         <v>110.96862400000001</v>
       </c>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-      <c r="AK24" s="1"/>
-      <c r="AL24" s="1"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
@@ -3873,8 +4184,8 @@
       <c r="BF24" s="1"/>
       <c r="BG24" s="1"/>
       <c r="BH24" s="1"/>
+      <c r="BI24" s="1"/>
       <c r="BJ24" s="1"/>
-      <c r="BK24" s="1"/>
       <c r="BL24" s="1"/>
       <c r="BM24" s="1"/>
       <c r="BN24" s="1"/>
@@ -3883,8 +4194,10 @@
       <c r="BQ24" s="1"/>
       <c r="BR24" s="1"/>
       <c r="BS24" s="1"/>
-    </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT24" s="1"/>
+      <c r="BU24" s="1"/>
+    </row>
+    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -3898,37 +4211,41 @@
       <c r="F25">
         <v>1</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25">
+        <v>300</v>
+      </c>
+      <c r="H25">
+        <v>1000</v>
+      </c>
+      <c r="I25" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4">
+      <c r="K25" s="4"/>
+      <c r="L25" s="4">
         <v>-12.120000000000005</v>
       </c>
-      <c r="K25" s="4">
+      <c r="M25" s="4">
         <v>1679.786106</v>
       </c>
-      <c r="L25" s="4">
+      <c r="N25" s="4">
         <v>509.64356400000003</v>
       </c>
-      <c r="M25" s="4">
+      <c r="O25" s="4">
         <v>489.064573</v>
       </c>
-      <c r="N25" s="4">
+      <c r="P25" s="4">
         <v>443.45080000000002</v>
       </c>
-      <c r="O25" s="4">
+      <c r="Q25" s="4">
         <v>396.19289099999997</v>
       </c>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-      <c r="AK25" s="1"/>
-      <c r="AL25" s="1"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
@@ -3951,8 +4268,8 @@
       <c r="BF25" s="1"/>
       <c r="BG25" s="1"/>
       <c r="BH25" s="1"/>
+      <c r="BI25" s="1"/>
       <c r="BJ25" s="1"/>
-      <c r="BK25" s="1"/>
       <c r="BL25" s="1"/>
       <c r="BM25" s="1"/>
       <c r="BN25" s="1"/>
@@ -3961,8 +4278,10 @@
       <c r="BQ25" s="1"/>
       <c r="BR25" s="1"/>
       <c r="BS25" s="1"/>
-    </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT25" s="1"/>
+      <c r="BU25" s="1"/>
+    </row>
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3973,37 +4292,41 @@
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26">
+        <v>300</v>
+      </c>
+      <c r="H26">
+        <v>1000</v>
+      </c>
+      <c r="I26" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4">
+      <c r="K26" s="4"/>
+      <c r="L26" s="4">
         <v>-16.799999999999955</v>
       </c>
-      <c r="K26" s="4">
+      <c r="M26" s="4">
         <v>549.17255799999998</v>
       </c>
-      <c r="L26" s="4">
+      <c r="N26" s="4">
         <v>496.630066</v>
       </c>
-      <c r="M26" s="4">
+      <c r="O26" s="4">
         <v>436.16551199999998</v>
       </c>
-      <c r="N26" s="4">
+      <c r="P26" s="4">
         <v>418.36746199999999</v>
       </c>
-      <c r="O26" s="4">
+      <c r="Q26" s="4">
         <v>391.94338199999999</v>
       </c>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="AK26" s="1"/>
-      <c r="AL26" s="1"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
@@ -4026,8 +4349,8 @@
       <c r="BF26" s="1"/>
       <c r="BG26" s="1"/>
       <c r="BH26" s="1"/>
+      <c r="BI26" s="1"/>
       <c r="BJ26" s="1"/>
-      <c r="BK26" s="1"/>
       <c r="BL26" s="1"/>
       <c r="BM26" s="1"/>
       <c r="BN26" s="1"/>
@@ -4036,8 +4359,10 @@
       <c r="BQ26" s="1"/>
       <c r="BR26" s="1"/>
       <c r="BS26" s="1"/>
-    </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT26" s="1"/>
+      <c r="BU26" s="1"/>
+    </row>
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -4045,16 +4370,20 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27">
+        <v>300</v>
+      </c>
+      <c r="H27">
+        <v>1000</v>
+      </c>
+      <c r="I27" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -4066,9 +4395,9 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-      <c r="W27" s="1"/>
-      <c r="AK27" s="1"/>
-      <c r="AL27" s="1"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="1"/>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
@@ -4091,8 +4420,8 @@
       <c r="BF27" s="1"/>
       <c r="BG27" s="1"/>
       <c r="BH27" s="1"/>
+      <c r="BI27" s="1"/>
       <c r="BJ27" s="1"/>
-      <c r="BK27" s="1"/>
       <c r="BL27" s="1"/>
       <c r="BM27" s="1"/>
       <c r="BN27" s="1"/>
@@ -4101,8 +4430,10 @@
       <c r="BQ27" s="1"/>
       <c r="BR27" s="1"/>
       <c r="BS27" s="1"/>
-    </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT27" s="1"/>
+      <c r="BU27" s="1"/>
+    </row>
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4115,11 +4446,15 @@
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28">
+        <v>300</v>
+      </c>
+      <c r="H28">
+        <v>1000</v>
+      </c>
+      <c r="I28" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -4131,9 +4466,9 @@
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
-      <c r="W28" s="1"/>
-      <c r="AK28" s="1"/>
-      <c r="AL28" s="1"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="1"/>
       <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
@@ -4156,8 +4491,8 @@
       <c r="BF28" s="1"/>
       <c r="BG28" s="1"/>
       <c r="BH28" s="1"/>
+      <c r="BI28" s="1"/>
       <c r="BJ28" s="1"/>
-      <c r="BK28" s="1"/>
       <c r="BL28" s="1"/>
       <c r="BM28" s="1"/>
       <c r="BN28" s="1"/>
@@ -4166,12 +4501,14 @@
       <c r="BQ28" s="1"/>
       <c r="BR28" s="1"/>
       <c r="BS28" s="1"/>
-    </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT28" s="1"/>
+      <c r="BU28" s="1"/>
+    </row>
+    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="AK29" s="1"/>
-      <c r="AL29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
       <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
@@ -4194,8 +4531,8 @@
       <c r="BF29" s="1"/>
       <c r="BG29" s="1"/>
       <c r="BH29" s="1"/>
+      <c r="BI29" s="1"/>
       <c r="BJ29" s="1"/>
-      <c r="BK29" s="1"/>
       <c r="BL29" s="1"/>
       <c r="BM29" s="1"/>
       <c r="BN29" s="1"/>
@@ -4204,12 +4541,14 @@
       <c r="BQ29" s="1"/>
       <c r="BR29" s="1"/>
       <c r="BS29" s="1"/>
-    </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT29" s="1"/>
+      <c r="BU29" s="1"/>
+    </row>
+    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="AK30" s="1"/>
-      <c r="AL30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
@@ -4232,8 +4571,8 @@
       <c r="BF30" s="1"/>
       <c r="BG30" s="1"/>
       <c r="BH30" s="1"/>
+      <c r="BI30" s="1"/>
       <c r="BJ30" s="1"/>
-      <c r="BK30" s="1"/>
       <c r="BL30" s="1"/>
       <c r="BM30" s="1"/>
       <c r="BN30" s="1"/>
@@ -4242,12 +4581,14 @@
       <c r="BQ30" s="1"/>
       <c r="BR30" s="1"/>
       <c r="BS30" s="1"/>
-    </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT30" s="1"/>
+      <c r="BU30" s="1"/>
+    </row>
+    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="AK31" s="1"/>
-      <c r="AL31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
@@ -4270,8 +4611,8 @@
       <c r="BF31" s="1"/>
       <c r="BG31" s="1"/>
       <c r="BH31" s="1"/>
+      <c r="BI31" s="1"/>
       <c r="BJ31" s="1"/>
-      <c r="BK31" s="1"/>
       <c r="BL31" s="1"/>
       <c r="BM31" s="1"/>
       <c r="BN31" s="1"/>
@@ -4280,12 +4621,14 @@
       <c r="BQ31" s="1"/>
       <c r="BR31" s="1"/>
       <c r="BS31" s="1"/>
-    </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT31" s="1"/>
+      <c r="BU31" s="1"/>
+    </row>
+    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="AK32" s="1"/>
-      <c r="AL32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
       <c r="AO32" s="1"/>
@@ -4308,8 +4651,8 @@
       <c r="BF32" s="1"/>
       <c r="BG32" s="1"/>
       <c r="BH32" s="1"/>
+      <c r="BI32" s="1"/>
       <c r="BJ32" s="1"/>
-      <c r="BK32" s="1"/>
       <c r="BL32" s="1"/>
       <c r="BM32" s="1"/>
       <c r="BN32" s="1"/>
@@ -4318,12 +4661,14 @@
       <c r="BQ32" s="1"/>
       <c r="BR32" s="1"/>
       <c r="BS32" s="1"/>
-    </row>
-    <row r="33" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT32" s="1"/>
+      <c r="BU32" s="1"/>
+    </row>
+    <row r="33" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="AK33" s="1"/>
-      <c r="AL33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
@@ -4346,8 +4691,8 @@
       <c r="BF33" s="1"/>
       <c r="BG33" s="1"/>
       <c r="BH33" s="1"/>
+      <c r="BI33" s="1"/>
       <c r="BJ33" s="1"/>
-      <c r="BK33" s="1"/>
       <c r="BL33" s="1"/>
       <c r="BM33" s="1"/>
       <c r="BN33" s="1"/>
@@ -4356,12 +4701,14 @@
       <c r="BQ33" s="1"/>
       <c r="BR33" s="1"/>
       <c r="BS33" s="1"/>
-    </row>
-    <row r="34" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT33" s="1"/>
+      <c r="BU33" s="1"/>
+    </row>
+    <row r="34" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="AK34" s="1"/>
-      <c r="AL34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
       <c r="AO34" s="1"/>
@@ -4384,8 +4731,8 @@
       <c r="BF34" s="1"/>
       <c r="BG34" s="1"/>
       <c r="BH34" s="1"/>
+      <c r="BI34" s="1"/>
       <c r="BJ34" s="1"/>
-      <c r="BK34" s="1"/>
       <c r="BL34" s="1"/>
       <c r="BM34" s="1"/>
       <c r="BN34" s="1"/>
@@ -4394,12 +4741,14 @@
       <c r="BQ34" s="1"/>
       <c r="BR34" s="1"/>
       <c r="BS34" s="1"/>
-    </row>
-    <row r="35" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT34" s="1"/>
+      <c r="BU34" s="1"/>
+    </row>
+    <row r="35" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="AK35" s="1"/>
-      <c r="AL35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
@@ -4422,8 +4771,8 @@
       <c r="BF35" s="1"/>
       <c r="BG35" s="1"/>
       <c r="BH35" s="1"/>
+      <c r="BI35" s="1"/>
       <c r="BJ35" s="1"/>
-      <c r="BK35" s="1"/>
       <c r="BL35" s="1"/>
       <c r="BM35" s="1"/>
       <c r="BN35" s="1"/>
@@ -4432,12 +4781,14 @@
       <c r="BQ35" s="1"/>
       <c r="BR35" s="1"/>
       <c r="BS35" s="1"/>
-    </row>
-    <row r="36" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT35" s="1"/>
+      <c r="BU35" s="1"/>
+    </row>
+    <row r="36" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="AK36" s="1"/>
-      <c r="AL36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
@@ -4460,8 +4811,8 @@
       <c r="BF36" s="1"/>
       <c r="BG36" s="1"/>
       <c r="BH36" s="1"/>
+      <c r="BI36" s="1"/>
       <c r="BJ36" s="1"/>
-      <c r="BK36" s="1"/>
       <c r="BL36" s="1"/>
       <c r="BM36" s="1"/>
       <c r="BN36" s="1"/>
@@ -4470,12 +4821,14 @@
       <c r="BQ36" s="1"/>
       <c r="BR36" s="1"/>
       <c r="BS36" s="1"/>
-    </row>
-    <row r="37" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT36" s="1"/>
+      <c r="BU36" s="1"/>
+    </row>
+    <row r="37" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="AK37" s="1"/>
-      <c r="AL37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
@@ -4498,8 +4851,8 @@
       <c r="BF37" s="1"/>
       <c r="BG37" s="1"/>
       <c r="BH37" s="1"/>
+      <c r="BI37" s="1"/>
       <c r="BJ37" s="1"/>
-      <c r="BK37" s="1"/>
       <c r="BL37" s="1"/>
       <c r="BM37" s="1"/>
       <c r="BN37" s="1"/>
@@ -4508,12 +4861,14 @@
       <c r="BQ37" s="1"/>
       <c r="BR37" s="1"/>
       <c r="BS37" s="1"/>
-    </row>
-    <row r="38" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT37" s="1"/>
+      <c r="BU37" s="1"/>
+    </row>
+    <row r="38" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="AK38" s="1"/>
-      <c r="AL38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
       <c r="AO38" s="1"/>
@@ -4536,8 +4891,8 @@
       <c r="BF38" s="1"/>
       <c r="BG38" s="1"/>
       <c r="BH38" s="1"/>
+      <c r="BI38" s="1"/>
       <c r="BJ38" s="1"/>
-      <c r="BK38" s="1"/>
       <c r="BL38" s="1"/>
       <c r="BM38" s="1"/>
       <c r="BN38" s="1"/>
@@ -4546,12 +4901,14 @@
       <c r="BQ38" s="1"/>
       <c r="BR38" s="1"/>
       <c r="BS38" s="1"/>
-    </row>
-    <row r="39" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT38" s="1"/>
+      <c r="BU38" s="1"/>
+    </row>
+    <row r="39" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="AK39" s="1"/>
-      <c r="AL39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
@@ -4574,8 +4931,8 @@
       <c r="BF39" s="1"/>
       <c r="BG39" s="1"/>
       <c r="BH39" s="1"/>
+      <c r="BI39" s="1"/>
       <c r="BJ39" s="1"/>
-      <c r="BK39" s="1"/>
       <c r="BL39" s="1"/>
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
@@ -4584,12 +4941,14 @@
       <c r="BQ39" s="1"/>
       <c r="BR39" s="1"/>
       <c r="BS39" s="1"/>
-    </row>
-    <row r="40" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT39" s="1"/>
+      <c r="BU39" s="1"/>
+    </row>
+    <row r="40" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="AK40" s="1"/>
-      <c r="AL40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
       <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
       <c r="AO40" s="1"/>
@@ -4612,8 +4971,8 @@
       <c r="BF40" s="1"/>
       <c r="BG40" s="1"/>
       <c r="BH40" s="1"/>
+      <c r="BI40" s="1"/>
       <c r="BJ40" s="1"/>
-      <c r="BK40" s="1"/>
       <c r="BL40" s="1"/>
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
@@ -4622,12 +4981,14 @@
       <c r="BQ40" s="1"/>
       <c r="BR40" s="1"/>
       <c r="BS40" s="1"/>
-    </row>
-    <row r="41" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT40" s="1"/>
+      <c r="BU40" s="1"/>
+    </row>
+    <row r="41" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="AK41" s="1"/>
-      <c r="AL41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
       <c r="AO41" s="1"/>
@@ -4650,8 +5011,8 @@
       <c r="BF41" s="1"/>
       <c r="BG41" s="1"/>
       <c r="BH41" s="1"/>
+      <c r="BI41" s="1"/>
       <c r="BJ41" s="1"/>
-      <c r="BK41" s="1"/>
       <c r="BL41" s="1"/>
       <c r="BM41" s="1"/>
       <c r="BN41" s="1"/>
@@ -4660,12 +5021,14 @@
       <c r="BQ41" s="1"/>
       <c r="BR41" s="1"/>
       <c r="BS41" s="1"/>
-    </row>
-    <row r="42" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT41" s="1"/>
+      <c r="BU41" s="1"/>
+    </row>
+    <row r="42" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="AK42" s="1"/>
-      <c r="AL42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
       <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
       <c r="AO42" s="1"/>
@@ -4688,8 +5051,8 @@
       <c r="BF42" s="1"/>
       <c r="BG42" s="1"/>
       <c r="BH42" s="1"/>
+      <c r="BI42" s="1"/>
       <c r="BJ42" s="1"/>
-      <c r="BK42" s="1"/>
       <c r="BL42" s="1"/>
       <c r="BM42" s="1"/>
       <c r="BN42" s="1"/>
@@ -4698,12 +5061,14 @@
       <c r="BQ42" s="1"/>
       <c r="BR42" s="1"/>
       <c r="BS42" s="1"/>
-    </row>
-    <row r="43" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT42" s="1"/>
+      <c r="BU42" s="1"/>
+    </row>
+    <row r="43" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="AK43" s="1"/>
-      <c r="AL43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
       <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
       <c r="AO43" s="1"/>
@@ -4726,8 +5091,8 @@
       <c r="BF43" s="1"/>
       <c r="BG43" s="1"/>
       <c r="BH43" s="1"/>
+      <c r="BI43" s="1"/>
       <c r="BJ43" s="1"/>
-      <c r="BK43" s="1"/>
       <c r="BL43" s="1"/>
       <c r="BM43" s="1"/>
       <c r="BN43" s="1"/>
@@ -4736,12 +5101,14 @@
       <c r="BQ43" s="1"/>
       <c r="BR43" s="1"/>
       <c r="BS43" s="1"/>
-    </row>
-    <row r="44" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT43" s="1"/>
+      <c r="BU43" s="1"/>
+    </row>
+    <row r="44" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="AK44" s="1"/>
-      <c r="AL44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
       <c r="AM44" s="1"/>
       <c r="AN44" s="1"/>
       <c r="AO44" s="1"/>
@@ -4764,8 +5131,8 @@
       <c r="BF44" s="1"/>
       <c r="BG44" s="1"/>
       <c r="BH44" s="1"/>
+      <c r="BI44" s="1"/>
       <c r="BJ44" s="1"/>
-      <c r="BK44" s="1"/>
       <c r="BL44" s="1"/>
       <c r="BM44" s="1"/>
       <c r="BN44" s="1"/>
@@ -4774,12 +5141,14 @@
       <c r="BQ44" s="1"/>
       <c r="BR44" s="1"/>
       <c r="BS44" s="1"/>
-    </row>
-    <row r="45" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT44" s="1"/>
+      <c r="BU44" s="1"/>
+    </row>
+    <row r="45" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="AK45" s="1"/>
-      <c r="AL45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
       <c r="AO45" s="1"/>
@@ -4802,8 +5171,8 @@
       <c r="BF45" s="1"/>
       <c r="BG45" s="1"/>
       <c r="BH45" s="1"/>
+      <c r="BI45" s="1"/>
       <c r="BJ45" s="1"/>
-      <c r="BK45" s="1"/>
       <c r="BL45" s="1"/>
       <c r="BM45" s="1"/>
       <c r="BN45" s="1"/>
@@ -4812,12 +5181,14 @@
       <c r="BQ45" s="1"/>
       <c r="BR45" s="1"/>
       <c r="BS45" s="1"/>
-    </row>
-    <row r="46" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT45" s="1"/>
+      <c r="BU45" s="1"/>
+    </row>
+    <row r="46" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="AK46" s="1"/>
-      <c r="AL46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
       <c r="AO46" s="1"/>
@@ -4840,8 +5211,8 @@
       <c r="BF46" s="1"/>
       <c r="BG46" s="1"/>
       <c r="BH46" s="1"/>
+      <c r="BI46" s="1"/>
       <c r="BJ46" s="1"/>
-      <c r="BK46" s="1"/>
       <c r="BL46" s="1"/>
       <c r="BM46" s="1"/>
       <c r="BN46" s="1"/>
@@ -4850,12 +5221,14 @@
       <c r="BQ46" s="1"/>
       <c r="BR46" s="1"/>
       <c r="BS46" s="1"/>
-    </row>
-    <row r="47" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT46" s="1"/>
+      <c r="BU46" s="1"/>
+    </row>
+    <row r="47" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="AK47" s="1"/>
-      <c r="AL47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
       <c r="AO47" s="1"/>
@@ -4878,8 +5251,8 @@
       <c r="BF47" s="1"/>
       <c r="BG47" s="1"/>
       <c r="BH47" s="1"/>
+      <c r="BI47" s="1"/>
       <c r="BJ47" s="1"/>
-      <c r="BK47" s="1"/>
       <c r="BL47" s="1"/>
       <c r="BM47" s="1"/>
       <c r="BN47" s="1"/>
@@ -4888,12 +5261,14 @@
       <c r="BQ47" s="1"/>
       <c r="BR47" s="1"/>
       <c r="BS47" s="1"/>
-    </row>
-    <row r="48" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT47" s="1"/>
+      <c r="BU47" s="1"/>
+    </row>
+    <row r="48" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="AK48" s="1"/>
-      <c r="AL48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
@@ -4916,8 +5291,8 @@
       <c r="BF48" s="1"/>
       <c r="BG48" s="1"/>
       <c r="BH48" s="1"/>
+      <c r="BI48" s="1"/>
       <c r="BJ48" s="1"/>
-      <c r="BK48" s="1"/>
       <c r="BL48" s="1"/>
       <c r="BM48" s="1"/>
       <c r="BN48" s="1"/>
@@ -4926,12 +5301,14 @@
       <c r="BQ48" s="1"/>
       <c r="BR48" s="1"/>
       <c r="BS48" s="1"/>
-    </row>
-    <row r="49" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT48" s="1"/>
+      <c r="BU48" s="1"/>
+    </row>
+    <row r="49" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="AK49" s="1"/>
-      <c r="AL49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
@@ -4954,8 +5331,8 @@
       <c r="BF49" s="1"/>
       <c r="BG49" s="1"/>
       <c r="BH49" s="1"/>
+      <c r="BI49" s="1"/>
       <c r="BJ49" s="1"/>
-      <c r="BK49" s="1"/>
       <c r="BL49" s="1"/>
       <c r="BM49" s="1"/>
       <c r="BN49" s="1"/>
@@ -4964,12 +5341,14 @@
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="1"/>
-    </row>
-    <row r="50" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT49" s="1"/>
+      <c r="BU49" s="1"/>
+    </row>
+    <row r="50" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="AK50" s="1"/>
-      <c r="AL50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
       <c r="AO50" s="1"/>
@@ -4992,8 +5371,8 @@
       <c r="BF50" s="1"/>
       <c r="BG50" s="1"/>
       <c r="BH50" s="1"/>
+      <c r="BI50" s="1"/>
       <c r="BJ50" s="1"/>
-      <c r="BK50" s="1"/>
       <c r="BL50" s="1"/>
       <c r="BM50" s="1"/>
       <c r="BN50" s="1"/>
@@ -5002,12 +5381,14 @@
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="1"/>
-    </row>
-    <row r="51" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT50" s="1"/>
+      <c r="BU50" s="1"/>
+    </row>
+    <row r="51" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="AK51" s="1"/>
-      <c r="AL51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
       <c r="AO51" s="1"/>
@@ -5030,8 +5411,8 @@
       <c r="BF51" s="1"/>
       <c r="BG51" s="1"/>
       <c r="BH51" s="1"/>
+      <c r="BI51" s="1"/>
       <c r="BJ51" s="1"/>
-      <c r="BK51" s="1"/>
       <c r="BL51" s="1"/>
       <c r="BM51" s="1"/>
       <c r="BN51" s="1"/>
@@ -5040,12 +5421,14 @@
       <c r="BQ51" s="1"/>
       <c r="BR51" s="1"/>
       <c r="BS51" s="1"/>
-    </row>
-    <row r="52" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT51" s="1"/>
+      <c r="BU51" s="1"/>
+    </row>
+    <row r="52" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="AK52" s="1"/>
-      <c r="AL52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
@@ -5068,8 +5451,8 @@
       <c r="BF52" s="1"/>
       <c r="BG52" s="1"/>
       <c r="BH52" s="1"/>
+      <c r="BI52" s="1"/>
       <c r="BJ52" s="1"/>
-      <c r="BK52" s="1"/>
       <c r="BL52" s="1"/>
       <c r="BM52" s="1"/>
       <c r="BN52" s="1"/>
@@ -5078,12 +5461,14 @@
       <c r="BQ52" s="1"/>
       <c r="BR52" s="1"/>
       <c r="BS52" s="1"/>
-    </row>
-    <row r="53" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT52" s="1"/>
+      <c r="BU52" s="1"/>
+    </row>
+    <row r="53" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="AK53" s="1"/>
-      <c r="AL53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
@@ -5106,8 +5491,8 @@
       <c r="BF53" s="1"/>
       <c r="BG53" s="1"/>
       <c r="BH53" s="1"/>
+      <c r="BI53" s="1"/>
       <c r="BJ53" s="1"/>
-      <c r="BK53" s="1"/>
       <c r="BL53" s="1"/>
       <c r="BM53" s="1"/>
       <c r="BN53" s="1"/>
@@ -5116,12 +5501,14 @@
       <c r="BQ53" s="1"/>
       <c r="BR53" s="1"/>
       <c r="BS53" s="1"/>
-    </row>
-    <row r="54" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT53" s="1"/>
+      <c r="BU53" s="1"/>
+    </row>
+    <row r="54" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="AK54" s="1"/>
-      <c r="AL54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
@@ -5144,8 +5531,8 @@
       <c r="BF54" s="1"/>
       <c r="BG54" s="1"/>
       <c r="BH54" s="1"/>
+      <c r="BI54" s="1"/>
       <c r="BJ54" s="1"/>
-      <c r="BK54" s="1"/>
       <c r="BL54" s="1"/>
       <c r="BM54" s="1"/>
       <c r="BN54" s="1"/>
@@ -5154,12 +5541,14 @@
       <c r="BQ54" s="1"/>
       <c r="BR54" s="1"/>
       <c r="BS54" s="1"/>
-    </row>
-    <row r="55" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT54" s="1"/>
+      <c r="BU54" s="1"/>
+    </row>
+    <row r="55" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="AK55" s="1"/>
-      <c r="AL55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
       <c r="AO55" s="1"/>
@@ -5182,8 +5571,8 @@
       <c r="BF55" s="1"/>
       <c r="BG55" s="1"/>
       <c r="BH55" s="1"/>
+      <c r="BI55" s="1"/>
       <c r="BJ55" s="1"/>
-      <c r="BK55" s="1"/>
       <c r="BL55" s="1"/>
       <c r="BM55" s="1"/>
       <c r="BN55" s="1"/>
@@ -5192,12 +5581,14 @@
       <c r="BQ55" s="1"/>
       <c r="BR55" s="1"/>
       <c r="BS55" s="1"/>
-    </row>
-    <row r="56" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT55" s="1"/>
+      <c r="BU55" s="1"/>
+    </row>
+    <row r="56" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="AK56" s="1"/>
-      <c r="AL56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
       <c r="AO56" s="1"/>
@@ -5220,8 +5611,8 @@
       <c r="BF56" s="1"/>
       <c r="BG56" s="1"/>
       <c r="BH56" s="1"/>
+      <c r="BI56" s="1"/>
       <c r="BJ56" s="1"/>
-      <c r="BK56" s="1"/>
       <c r="BL56" s="1"/>
       <c r="BM56" s="1"/>
       <c r="BN56" s="1"/>
@@ -5230,12 +5621,14 @@
       <c r="BQ56" s="1"/>
       <c r="BR56" s="1"/>
       <c r="BS56" s="1"/>
-    </row>
-    <row r="57" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT56" s="1"/>
+      <c r="BU56" s="1"/>
+    </row>
+    <row r="57" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="AK57" s="1"/>
-      <c r="AL57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
       <c r="AO57" s="1"/>
@@ -5258,8 +5651,8 @@
       <c r="BF57" s="1"/>
       <c r="BG57" s="1"/>
       <c r="BH57" s="1"/>
+      <c r="BI57" s="1"/>
       <c r="BJ57" s="1"/>
-      <c r="BK57" s="1"/>
       <c r="BL57" s="1"/>
       <c r="BM57" s="1"/>
       <c r="BN57" s="1"/>
@@ -5268,12 +5661,14 @@
       <c r="BQ57" s="1"/>
       <c r="BR57" s="1"/>
       <c r="BS57" s="1"/>
-    </row>
-    <row r="58" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT57" s="1"/>
+      <c r="BU57" s="1"/>
+    </row>
+    <row r="58" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="AK58" s="1"/>
-      <c r="AL58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
       <c r="AO58" s="1"/>
@@ -5296,8 +5691,8 @@
       <c r="BF58" s="1"/>
       <c r="BG58" s="1"/>
       <c r="BH58" s="1"/>
+      <c r="BI58" s="1"/>
       <c r="BJ58" s="1"/>
-      <c r="BK58" s="1"/>
       <c r="BL58" s="1"/>
       <c r="BM58" s="1"/>
       <c r="BN58" s="1"/>
@@ -5306,12 +5701,14 @@
       <c r="BQ58" s="1"/>
       <c r="BR58" s="1"/>
       <c r="BS58" s="1"/>
-    </row>
-    <row r="59" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT58" s="1"/>
+      <c r="BU58" s="1"/>
+    </row>
+    <row r="59" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="AK59" s="1"/>
-      <c r="AL59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
       <c r="AO59" s="1"/>
@@ -5334,8 +5731,8 @@
       <c r="BF59" s="1"/>
       <c r="BG59" s="1"/>
       <c r="BH59" s="1"/>
+      <c r="BI59" s="1"/>
       <c r="BJ59" s="1"/>
-      <c r="BK59" s="1"/>
       <c r="BL59" s="1"/>
       <c r="BM59" s="1"/>
       <c r="BN59" s="1"/>
@@ -5344,12 +5741,14 @@
       <c r="BQ59" s="1"/>
       <c r="BR59" s="1"/>
       <c r="BS59" s="1"/>
-    </row>
-    <row r="60" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT59" s="1"/>
+      <c r="BU59" s="1"/>
+    </row>
+    <row r="60" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="AK60" s="1"/>
-      <c r="AL60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
       <c r="AO60" s="1"/>
@@ -5372,8 +5771,8 @@
       <c r="BF60" s="1"/>
       <c r="BG60" s="1"/>
       <c r="BH60" s="1"/>
+      <c r="BI60" s="1"/>
       <c r="BJ60" s="1"/>
-      <c r="BK60" s="1"/>
       <c r="BL60" s="1"/>
       <c r="BM60" s="1"/>
       <c r="BN60" s="1"/>
@@ -5382,12 +5781,14 @@
       <c r="BQ60" s="1"/>
       <c r="BR60" s="1"/>
       <c r="BS60" s="1"/>
-    </row>
-    <row r="61" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT60" s="1"/>
+      <c r="BU60" s="1"/>
+    </row>
+    <row r="61" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="AK61" s="1"/>
-      <c r="AL61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
       <c r="AO61" s="1"/>
@@ -5410,8 +5811,8 @@
       <c r="BF61" s="1"/>
       <c r="BG61" s="1"/>
       <c r="BH61" s="1"/>
+      <c r="BI61" s="1"/>
       <c r="BJ61" s="1"/>
-      <c r="BK61" s="1"/>
       <c r="BL61" s="1"/>
       <c r="BM61" s="1"/>
       <c r="BN61" s="1"/>
@@ -5420,12 +5821,14 @@
       <c r="BQ61" s="1"/>
       <c r="BR61" s="1"/>
       <c r="BS61" s="1"/>
-    </row>
-    <row r="62" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT61" s="1"/>
+      <c r="BU61" s="1"/>
+    </row>
+    <row r="62" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="AK62" s="1"/>
-      <c r="AL62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
       <c r="AM62" s="1"/>
       <c r="AN62" s="1"/>
       <c r="AO62" s="1"/>
@@ -5448,8 +5851,8 @@
       <c r="BF62" s="1"/>
       <c r="BG62" s="1"/>
       <c r="BH62" s="1"/>
+      <c r="BI62" s="1"/>
       <c r="BJ62" s="1"/>
-      <c r="BK62" s="1"/>
       <c r="BL62" s="1"/>
       <c r="BM62" s="1"/>
       <c r="BN62" s="1"/>
@@ -5458,12 +5861,14 @@
       <c r="BQ62" s="1"/>
       <c r="BR62" s="1"/>
       <c r="BS62" s="1"/>
-    </row>
-    <row r="63" spans="5:71" x14ac:dyDescent="0.25">
+      <c r="BT62" s="1"/>
+      <c r="BU62" s="1"/>
+    </row>
+    <row r="63" spans="5:73" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="AK63" s="1"/>
-      <c r="AL63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
       <c r="AM63" s="1"/>
       <c r="AN63" s="1"/>
       <c r="AO63" s="1"/>
@@ -5486,8 +5891,8 @@
       <c r="BF63" s="1"/>
       <c r="BG63" s="1"/>
       <c r="BH63" s="1"/>
+      <c r="BI63" s="1"/>
       <c r="BJ63" s="1"/>
-      <c r="BK63" s="1"/>
       <c r="BL63" s="1"/>
       <c r="BM63" s="1"/>
       <c r="BN63" s="1"/>
@@ -5496,6 +5901,8 @@
       <c r="BQ63" s="1"/>
       <c r="BR63" s="1"/>
       <c r="BS63" s="1"/>
+      <c r="BT63" s="1"/>
+      <c r="BU63" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5504,6 +5911,230 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056B77A4-B8AE-40D4-A168-746976D372E2}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>900</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1500</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="M3" s="8">
+        <v>1E-10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6459F932-8E59-4309-B8D3-B0D97D611334}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA3BA1A-334E-44D2-96CB-219546C8DBF5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5530,24 +6161,24 @@
         <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>0.28999999999999998</v>
@@ -5556,15 +6187,15 @@
         <v>23.23</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>0.52</v>
@@ -5573,15 +6204,15 @@
         <v>19.78</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5">
         <v>0.71</v>
@@ -5590,10 +6221,10 @@
         <v>23.69</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -5601,11 +6232,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -5641,13 +6272,13 @@
         <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>57</v>
@@ -5725,7 +6356,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
@@ -5743,7 +6374,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5752,7 +6383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -5760,7 +6391,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5780,7 +6411,7 @@
         <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5791,83 +6422,97 @@
         <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5876,7 +6521,9 @@
       <c r="B10" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -5885,7 +6532,9 @@
       <c r="B11" t="b">
         <v>1</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -5894,43 +6543,51 @@
       <c r="B12" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="9"/>
+        <v>117</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -5939,7 +6596,9 @@
       <c r="B16" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5947,7 +6606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -5990,10 +6649,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -6004,10 +6663,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6018,10 +6677,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -6032,10 +6691,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -6046,10 +6705,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>0</v>

</xml_diff>

<commit_message>
Updated OpenMKM IO functionality
Added option to change activation function for adsorption reactions.
By default, beta will be set to 0 for adsorption, 1 for surface reactions.
Updated omkm example
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_dev\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A29F855-D91C-4F59-9343-BD912016FAC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A900271-0F4B-4F23-B968-6FD5BF9D51BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="576" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="183">
   <si>
     <t>name</t>
   </si>
@@ -583,6 +583,9 @@
   </si>
   <si>
     <t>atm</t>
+  </si>
+  <si>
+    <t>kcal</t>
   </si>
 </sst>
 </file>
@@ -1466,22 +1469,22 @@
       <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1570,7 @@
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1612,7 +1615,7 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>2744</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1759,7 +1762,7 @@
       <c r="G7" s="3"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1768,7 +1771,7 @@
       <c r="G8" s="3"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1777,7 +1780,7 @@
       <c r="G9" s="3"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1786,7 +1789,7 @@
       <c r="G10" s="3"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1795,7 +1798,7 @@
       <c r="G11" s="3"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1804,7 +1807,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1813,7 +1816,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1822,7 +1825,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1831,7 +1834,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1840,7 +1843,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1849,7 +1852,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1858,7 +1861,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1867,7 +1870,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1876,7 +1879,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1885,7 +1888,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1894,7 +1897,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1903,7 +1906,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1912,7 +1915,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1921,7 +1924,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1930,7 +1933,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1939,7 +1942,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1948,7 +1951,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1966,26 +1969,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BU63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H3" sqref="H3:H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2107,7 +2110,7 @@
       <c r="BT1" s="1"/>
       <c r="BU1" s="1"/>
     </row>
-    <row r="2" spans="1:73" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:73" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -2229,7 +2232,7 @@
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2320,7 +2323,7 @@
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2420,7 +2423,7 @@
       <c r="BT4" s="1"/>
       <c r="BU4" s="1"/>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2511,7 +2514,7 @@
       <c r="BT5" s="1"/>
       <c r="BU5" s="1"/>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -2609,7 +2612,7 @@
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -2703,7 +2706,7 @@
       <c r="BT7" s="1"/>
       <c r="BU7" s="1"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -2782,7 +2785,7 @@
       <c r="BT8" s="1"/>
       <c r="BU8" s="1"/>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -2882,7 +2885,7 @@
       <c r="BT9" s="1"/>
       <c r="BU9" s="1"/>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -2976,7 +2979,7 @@
       <c r="BT10" s="1"/>
       <c r="BU10" s="1"/>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -3064,7 +3067,7 @@
       <c r="BT11" s="1"/>
       <c r="BU11" s="1"/>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -3160,7 +3163,7 @@
       <c r="BT12" s="1"/>
       <c r="BU12" s="1"/>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -3250,7 +3253,7 @@
       <c r="BT13" s="1"/>
       <c r="BU13" s="1"/>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -3334,7 +3337,7 @@
       <c r="BT14" s="1"/>
       <c r="BU14" s="1"/>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>107</v>
       </c>
@@ -3415,7 +3418,7 @@
       <c r="BS15" s="1"/>
       <c r="BT15" s="1"/>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -3486,7 +3489,7 @@
       <c r="BT16" s="1"/>
       <c r="BU16" s="1"/>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -3571,7 +3574,7 @@
       <c r="BT17" s="1"/>
       <c r="BU17" s="1"/>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3650,7 +3653,7 @@
       <c r="BT18" s="1"/>
       <c r="BU18" s="1"/>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -3729,7 +3732,7 @@
       <c r="BT19" s="1"/>
       <c r="BU19" s="1"/>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3829,7 +3832,7 @@
       <c r="BT20" s="1"/>
       <c r="BU20" s="1"/>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -3923,7 +3926,7 @@
       <c r="BT21" s="1"/>
       <c r="BU21" s="1"/>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -4011,7 +4014,7 @@
       <c r="BT22" s="1"/>
       <c r="BU22" s="1"/>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -4107,7 +4110,7 @@
       <c r="BT23" s="1"/>
       <c r="BU23" s="1"/>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -4197,7 +4200,7 @@
       <c r="BT24" s="1"/>
       <c r="BU24" s="1"/>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -4281,7 +4284,7 @@
       <c r="BT25" s="1"/>
       <c r="BU25" s="1"/>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -4362,7 +4365,7 @@
       <c r="BT26" s="1"/>
       <c r="BU26" s="1"/>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -4433,7 +4436,7 @@
       <c r="BT27" s="1"/>
       <c r="BU27" s="1"/>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4504,7 +4507,7 @@
       <c r="BT28" s="1"/>
       <c r="BU28" s="1"/>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -4544,7 +4547,7 @@
       <c r="BT29" s="1"/>
       <c r="BU29" s="1"/>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -4584,7 +4587,7 @@
       <c r="BT30" s="1"/>
       <c r="BU30" s="1"/>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -4624,7 +4627,7 @@
       <c r="BT31" s="1"/>
       <c r="BU31" s="1"/>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -4664,7 +4667,7 @@
       <c r="BT32" s="1"/>
       <c r="BU32" s="1"/>
     </row>
-    <row r="33" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -4704,7 +4707,7 @@
       <c r="BT33" s="1"/>
       <c r="BU33" s="1"/>
     </row>
-    <row r="34" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -4744,7 +4747,7 @@
       <c r="BT34" s="1"/>
       <c r="BU34" s="1"/>
     </row>
-    <row r="35" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -4784,7 +4787,7 @@
       <c r="BT35" s="1"/>
       <c r="BU35" s="1"/>
     </row>
-    <row r="36" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -4824,7 +4827,7 @@
       <c r="BT36" s="1"/>
       <c r="BU36" s="1"/>
     </row>
-    <row r="37" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -4864,7 +4867,7 @@
       <c r="BT37" s="1"/>
       <c r="BU37" s="1"/>
     </row>
-    <row r="38" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -4904,7 +4907,7 @@
       <c r="BT38" s="1"/>
       <c r="BU38" s="1"/>
     </row>
-    <row r="39" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -4944,7 +4947,7 @@
       <c r="BT39" s="1"/>
       <c r="BU39" s="1"/>
     </row>
-    <row r="40" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -4984,7 +4987,7 @@
       <c r="BT40" s="1"/>
       <c r="BU40" s="1"/>
     </row>
-    <row r="41" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -5024,7 +5027,7 @@
       <c r="BT41" s="1"/>
       <c r="BU41" s="1"/>
     </row>
-    <row r="42" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -5064,7 +5067,7 @@
       <c r="BT42" s="1"/>
       <c r="BU42" s="1"/>
     </row>
-    <row r="43" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -5104,7 +5107,7 @@
       <c r="BT43" s="1"/>
       <c r="BU43" s="1"/>
     </row>
-    <row r="44" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -5144,7 +5147,7 @@
       <c r="BT44" s="1"/>
       <c r="BU44" s="1"/>
     </row>
-    <row r="45" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -5184,7 +5187,7 @@
       <c r="BT45" s="1"/>
       <c r="BU45" s="1"/>
     </row>
-    <row r="46" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -5224,7 +5227,7 @@
       <c r="BT46" s="1"/>
       <c r="BU46" s="1"/>
     </row>
-    <row r="47" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -5264,7 +5267,7 @@
       <c r="BT47" s="1"/>
       <c r="BU47" s="1"/>
     </row>
-    <row r="48" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -5304,7 +5307,7 @@
       <c r="BT48" s="1"/>
       <c r="BU48" s="1"/>
     </row>
-    <row r="49" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -5344,7 +5347,7 @@
       <c r="BT49" s="1"/>
       <c r="BU49" s="1"/>
     </row>
-    <row r="50" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -5384,7 +5387,7 @@
       <c r="BT50" s="1"/>
       <c r="BU50" s="1"/>
     </row>
-    <row r="51" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -5424,7 +5427,7 @@
       <c r="BT51" s="1"/>
       <c r="BU51" s="1"/>
     </row>
-    <row r="52" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -5464,7 +5467,7 @@
       <c r="BT52" s="1"/>
       <c r="BU52" s="1"/>
     </row>
-    <row r="53" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -5504,7 +5507,7 @@
       <c r="BT53" s="1"/>
       <c r="BU53" s="1"/>
     </row>
-    <row r="54" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -5544,7 +5547,7 @@
       <c r="BT54" s="1"/>
       <c r="BU54" s="1"/>
     </row>
-    <row r="55" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -5584,7 +5587,7 @@
       <c r="BT55" s="1"/>
       <c r="BU55" s="1"/>
     </row>
-    <row r="56" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -5624,7 +5627,7 @@
       <c r="BT56" s="1"/>
       <c r="BU56" s="1"/>
     </row>
-    <row r="57" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -5664,7 +5667,7 @@
       <c r="BT57" s="1"/>
       <c r="BU57" s="1"/>
     </row>
-    <row r="58" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -5704,7 +5707,7 @@
       <c r="BT58" s="1"/>
       <c r="BU58" s="1"/>
     </row>
-    <row r="59" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -5744,7 +5747,7 @@
       <c r="BT59" s="1"/>
       <c r="BU59" s="1"/>
     </row>
-    <row r="60" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -5784,7 +5787,7 @@
       <c r="BT60" s="1"/>
       <c r="BU60" s="1"/>
     </row>
-    <row r="61" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -5824,7 +5827,7 @@
       <c r="BT61" s="1"/>
       <c r="BU61" s="1"/>
     </row>
-    <row r="62" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -5864,7 +5867,7 @@
       <c r="BT62" s="1"/>
       <c r="BU62" s="1"/>
     </row>
-    <row r="63" spans="5:73" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:73" x14ac:dyDescent="0.3">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -5919,9 +5922,9 @@
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -5965,7 +5968,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>151</v>
       </c>
@@ -6009,7 +6012,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -6064,12 +6067,12 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>165</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>171</v>
       </c>
@@ -6109,7 +6112,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -6123,7 +6126,7 @@
         <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F3" t="s">
         <v>181</v>
@@ -6145,9 +6148,9 @@
       <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6164,7 +6167,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>87</v>
@@ -6176,7 +6179,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -6193,7 +6196,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -6210,7 +6213,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -6243,16 +6246,16 @@
       <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="9" width="9.5546875" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6284,7 +6287,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
@@ -6306,7 +6309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -6317,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -6331,7 +6334,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -6354,7 +6357,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -6391,16 +6394,16 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -6414,7 +6417,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -6428,7 +6431,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -6439,7 +6442,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -6450,7 +6453,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -6461,7 +6464,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -6489,7 +6492,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -6503,7 +6506,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -6514,7 +6517,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -6525,7 +6528,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -6536,7 +6539,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -6547,7 +6550,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -6561,7 +6564,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -6575,7 +6578,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -6589,7 +6592,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6608,18 +6611,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E12" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -6632,8 +6635,11 @@
       <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>77</v>
       </c>
@@ -6646,8 +6652,11 @@
       <c r="D2" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -6660,8 +6669,11 @@
       <c r="D3">
         <v>-52.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -6674,8 +6686,11 @@
       <c r="D4">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -6688,8 +6703,11 @@
       <c r="D5">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -6702,8 +6720,11 @@
       <c r="D6">
         <v>-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -6716,8 +6737,11 @@
       <c r="D7">
         <v>-20.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6730,8 +6754,11 @@
       <c r="D8">
         <v>-52.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -6744,8 +6771,11 @@
       <c r="D9">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -6758,8 +6788,11 @@
       <c r="D10">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -6772,8 +6805,11 @@
       <c r="D11">
         <v>-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -6785,6 +6821,9 @@
       </c>
       <c r="D12">
         <v>-20.7</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added option to arbitrarily set A and Ea in SurfaceReaction
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_dev\docs\source\examples_jupyter\omkm_io\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_master\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A900271-0F4B-4F23-B968-6FD5BF9D51BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DF0556-B4D4-43CC-A9AD-516413C6BEB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="187">
   <si>
     <t>name</t>
   </si>
@@ -586,6 +586,18 @@
   </si>
   <si>
     <t>kcal</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t>Manually specify pre-exponential constant.</t>
+  </si>
+  <si>
+    <t>Manully specify activation energy in kcal/mol</t>
   </si>
 </sst>
 </file>
@@ -6388,13 +6400,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6403,7 +6415,7 @@
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -6416,8 +6428,14 @@
       <c r="D1" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -6430,8 +6448,14 @@
       <c r="D2" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -6442,7 +6466,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -6453,7 +6477,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -6464,7 +6488,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -6477,8 +6501,14 @@
       <c r="D6" s="9" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="8">
+        <v>9.9999999999999998E+23</v>
+      </c>
+      <c r="F6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -6492,7 +6522,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -6506,7 +6536,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -6517,7 +6547,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -6528,7 +6558,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -6539,7 +6569,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -6550,7 +6580,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -6564,7 +6594,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -6578,7 +6608,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -6592,7 +6622,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6613,7 +6643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="182" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="E12" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated units for site density in OpenMKM_IO input spreadsheet
</commit_message>
<xml_diff>
--- a/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
+++ b/docs/source/examples_jupyter/omkm_io/inputs/NH3_Input_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_dev\docs\source\examples_jupyter\omkm_io\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Dropbox\UDelDocuments\UDelResearch\Github\pmutt_master\docs\source\examples_jupyter\omkm_io\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3B06F2-3361-40F9-B4C8-1116BC01FE94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A6E061-5049-4F62-9163-C5F30577755C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="9" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>Bulk density in g/cm3. Only required for StoichiometricSolid</t>
   </si>
   <si>
-    <t>Site density in molecule/cm2. Only required for InteractingInterface</t>
-  </si>
-  <si>
     <t>Type of phase</t>
   </si>
   <si>
@@ -622,6 +619,9 @@
   </si>
   <si>
     <t>Transition state used instead of BEP</t>
+  </si>
+  <si>
+    <t>Site density in mol/cm2. Only required for InteractingInterface</t>
   </si>
 </sst>
 </file>
@@ -1498,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6459F932-8E59-4309-B8D3-B0D97D611334}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1509,62 +1509,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
         <v>176</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>177</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>178</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" t="s">
         <v>179</v>
-      </c>
-      <c r="E3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1576,11 +1576,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC39740C-BBBA-4550-A14F-BA7A8AC6E618}">
   <dimension ref="A1:BD29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1609,7 +1609,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -2087,7 +2087,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X9" sqref="X9"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2113,19 +2113,19 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -2229,25 +2229,25 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>50</v>
@@ -2630,7 +2630,7 @@
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2822,7 +2822,7 @@
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3279,7 +3279,7 @@
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="14" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3534,7 +3534,7 @@
     </row>
     <row r="16" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3611,7 +3611,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -3696,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -3775,7 +3775,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -3957,7 +3957,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -4051,7 +4051,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -4487,7 +4487,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -6031,9 +6031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056B77A4-B8AE-40D4-A168-746976D372E2}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="204" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6044,98 +6044,98 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
         <v>146</v>
-      </c>
-      <c r="B3" t="s">
-        <v>147</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -6159,7 +6159,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K3" s="8">
         <v>1.0000000000000001E-15</v>
@@ -6171,7 +6171,7 @@
         <v>1E-10</v>
       </c>
       <c r="N3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -6188,7 +6188,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6198,33 +6198,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>0.28999999999999998</v>
@@ -6233,15 +6233,15 @@
         <v>23.23</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>0.52</v>
@@ -6250,15 +6250,15 @@
         <v>19.78</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5">
         <v>0.71</v>
@@ -6267,10 +6267,10 @@
         <v>23.69</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -6282,11 +6282,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6306,7 +6306,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>43</v>
@@ -6315,19 +6315,19 @@
         <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>57</v>
@@ -6338,28 +6338,28 @@
         <v>56</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>58</v>
@@ -6381,13 +6381,13 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4">
         <v>12.4</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -6395,7 +6395,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="8">
         <v>2.1671000000000001E-9</v>
@@ -6410,15 +6410,15 @@
         <v>1</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="8">
         <v>4.4385000000000002E-10</v>
@@ -6433,7 +6433,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -6446,11 +6446,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="235" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="260" zoomScaleNormal="235" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6467,19 +6467,19 @@
         <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6490,63 +6490,63 @@
         <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" s="8">
         <v>9.6E+17</v>
@@ -6555,46 +6555,46 @@
         <v>14.2</v>
       </c>
       <c r="G6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -6605,7 +6605,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -6616,7 +6616,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -6627,52 +6627,52 @@
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -6683,10 +6683,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -6697,10 +6697,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="182" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6709,46 +6709,49 @@
     <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -6760,12 +6763,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6777,12 +6780,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -6794,12 +6797,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -6811,12 +6814,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -6828,7 +6831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6845,7 +6848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -6862,7 +6865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -6879,7 +6882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -6896,7 +6899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>

</xml_diff>